<commit_message>
wrote bash script that uses spreadsheet info to update and open map
</commit_message>
<xml_diff>
--- a/map/map_data.xlsx
+++ b/map/map_data.xlsx
@@ -1,23 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22228"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="28209"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alex Ellison\Desktop\CodeForGood\map\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/britneyting/Desktop/Code for Good 2019-20/BrightonMarineMap/map/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B89F5C0-ACA1-4D41-A664-EC1B0997835E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="24496" windowHeight="15796" xr2:uid="{D5CD3BF6-7BDC-4B99-BDC7-1E82915A4C9A}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -2496,7 +2501,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -2564,59 +2569,59 @@
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2962,22 +2967,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CBE39C63-2E3D-4C18-AAF5-D0A4B6862FF8}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D352"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="19.9296875" customWidth="1"/>
-    <col min="2" max="2" width="18.19921875" customWidth="1"/>
-    <col min="3" max="3" width="18.59765625" customWidth="1"/>
-    <col min="4" max="4" width="29.19921875" customWidth="1"/>
+    <col min="1" max="1" width="20" customWidth="1"/>
+    <col min="2" max="2" width="18.1640625" customWidth="1"/>
+    <col min="3" max="3" width="18.6640625" customWidth="1"/>
+    <col min="4" max="4" width="29.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -2991,7 +2996,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="85.5" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:4" ht="90" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>4</v>
       </c>
@@ -3005,7 +3010,7 @@
         <v>22498</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="85.5" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:4" ht="75" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
         <v>6</v>
       </c>
@@ -3019,7 +3024,7 @@
         <v>29649</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="85.5" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:4" ht="90" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
         <v>8</v>
       </c>
@@ -3033,7 +3038,7 @@
         <v>21344</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:4" ht="75" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
         <v>10</v>
       </c>
@@ -3047,7 +3052,7 @@
         <v>29035</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="85.5" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:4" ht="90" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
         <v>12</v>
       </c>
@@ -3061,7 +3066,7 @@
         <v>25239</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:4" ht="75" x14ac:dyDescent="0.2">
       <c r="A7" s="6" t="s">
         <v>14</v>
       </c>
@@ -3075,7 +3080,7 @@
         <v>24364</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="57" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:4" ht="60" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
         <v>16</v>
       </c>
@@ -3089,7 +3094,7 @@
         <v>29250</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:4" ht="75" x14ac:dyDescent="0.2">
       <c r="A9" s="6" t="s">
         <v>18</v>
       </c>
@@ -3103,7 +3108,7 @@
         <v>23439</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="85.5" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:4" ht="90" x14ac:dyDescent="0.2">
       <c r="A10" s="6" t="s">
         <v>20</v>
       </c>
@@ -3117,7 +3122,7 @@
         <v>25323</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:4" ht="75" x14ac:dyDescent="0.2">
       <c r="A11" s="6" t="s">
         <v>22</v>
       </c>
@@ -3131,7 +3136,7 @@
         <v>26610</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="99.75" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:4" ht="90" x14ac:dyDescent="0.2">
       <c r="A12" s="6" t="s">
         <v>24</v>
       </c>
@@ -3145,7 +3150,7 @@
         <v>24955</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="85.5" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:4" ht="90" x14ac:dyDescent="0.2">
       <c r="A13" s="6" t="s">
         <v>26</v>
       </c>
@@ -3159,7 +3164,7 @@
         <v>22488</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="85.5" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:4" ht="90" x14ac:dyDescent="0.2">
       <c r="A14" s="6" t="s">
         <v>28</v>
       </c>
@@ -3173,7 +3178,7 @@
         <v>26633</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:4" ht="75" x14ac:dyDescent="0.2">
       <c r="A15" s="6" t="s">
         <v>30</v>
       </c>
@@ -3187,7 +3192,7 @@
         <v>22455</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:4" ht="75" x14ac:dyDescent="0.2">
       <c r="A16" s="6" t="s">
         <v>32</v>
       </c>
@@ -3201,7 +3206,7 @@
         <v>28885</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:4" ht="75" x14ac:dyDescent="0.2">
       <c r="A17" s="6" t="s">
         <v>34</v>
       </c>
@@ -3215,7 +3220,7 @@
         <v>24820</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:4" ht="75" x14ac:dyDescent="0.2">
       <c r="A18" s="6" t="s">
         <v>36</v>
       </c>
@@ -3229,7 +3234,7 @@
         <v>22148</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:4" ht="75" x14ac:dyDescent="0.2">
       <c r="A19" s="6" t="s">
         <v>38</v>
       </c>
@@ -3243,7 +3248,7 @@
         <v>25177</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="85.5" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:4" ht="90" x14ac:dyDescent="0.2">
       <c r="A20" s="6" t="s">
         <v>40</v>
       </c>
@@ -3257,7 +3262,7 @@
         <v>26312</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="57" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:4" ht="60" x14ac:dyDescent="0.2">
       <c r="A21" s="6" t="s">
         <v>42</v>
       </c>
@@ -3271,7 +3276,7 @@
         <v>25899</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="85.5" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:4" ht="90" x14ac:dyDescent="0.2">
       <c r="A22" s="6" t="s">
         <v>44</v>
       </c>
@@ -3285,7 +3290,7 @@
         <v>27099</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="57" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:4" ht="60" x14ac:dyDescent="0.2">
       <c r="A23" s="6" t="s">
         <v>46</v>
       </c>
@@ -3299,7 +3304,7 @@
         <v>24058</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="85.5" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:4" ht="90" x14ac:dyDescent="0.2">
       <c r="A24" s="6" t="s">
         <v>48</v>
       </c>
@@ -3313,7 +3318,7 @@
         <v>21739</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:4" ht="75" x14ac:dyDescent="0.2">
       <c r="A25" s="6" t="s">
         <v>50</v>
       </c>
@@ -3327,7 +3332,7 @@
         <v>28698</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:4" ht="75" x14ac:dyDescent="0.2">
       <c r="A26" s="6" t="s">
         <v>52</v>
       </c>
@@ -3341,7 +3346,7 @@
         <v>25292</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:4" ht="75" x14ac:dyDescent="0.2">
       <c r="A27" s="6" t="s">
         <v>54</v>
       </c>
@@ -3355,7 +3360,7 @@
         <v>24042</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="57" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:4" ht="60" x14ac:dyDescent="0.2">
       <c r="A28" s="6" t="s">
         <v>56</v>
       </c>
@@ -3369,7 +3374,7 @@
         <v>27944</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:4" ht="75" x14ac:dyDescent="0.2">
       <c r="A29" s="6" t="s">
         <v>58</v>
       </c>
@@ -3383,7 +3388,7 @@
         <v>25514</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:4" ht="75" x14ac:dyDescent="0.2">
       <c r="A30" s="6" t="s">
         <v>60</v>
       </c>
@@ -3397,7 +3402,7 @@
         <v>26391</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:4" ht="75" x14ac:dyDescent="0.2">
       <c r="A31" s="6" t="s">
         <v>62</v>
       </c>
@@ -3411,7 +3416,7 @@
         <v>28173</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="85.5" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:4" ht="90" x14ac:dyDescent="0.2">
       <c r="A32" s="6" t="s">
         <v>63</v>
       </c>
@@ -3425,7 +3430,7 @@
         <v>25548</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="85.5" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:4" ht="90" x14ac:dyDescent="0.2">
       <c r="A33" s="6" t="s">
         <v>65</v>
       </c>
@@ -3439,7 +3444,7 @@
         <v>28422</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:4" ht="75" x14ac:dyDescent="0.2">
       <c r="A34" s="6" t="s">
         <v>67</v>
       </c>
@@ -3453,7 +3458,7 @@
         <v>26724</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:4" ht="75" x14ac:dyDescent="0.2">
       <c r="A35" s="6" t="s">
         <v>69</v>
       </c>
@@ -3467,7 +3472,7 @@
         <v>25028</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:4" ht="75" x14ac:dyDescent="0.2">
       <c r="A36" s="6" t="s">
         <v>71</v>
       </c>
@@ -3481,7 +3486,7 @@
         <v>28119</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:4" ht="75" x14ac:dyDescent="0.2">
       <c r="A37" s="6" t="s">
         <v>73</v>
       </c>
@@ -3495,7 +3500,7 @@
         <v>28870</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="85.5" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:4" ht="90" x14ac:dyDescent="0.2">
       <c r="A38" s="6" t="s">
         <v>75</v>
       </c>
@@ -3509,7 +3514,7 @@
         <v>27297</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="85.5" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:4" ht="75" x14ac:dyDescent="0.2">
       <c r="A39" s="6" t="s">
         <v>76</v>
       </c>
@@ -3523,7 +3528,7 @@
         <v>29312</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:4" ht="75" x14ac:dyDescent="0.2">
       <c r="A40" s="6" t="s">
         <v>77</v>
       </c>
@@ -3537,7 +3542,7 @@
         <v>25535</v>
       </c>
     </row>
-    <row r="41" spans="1:4" ht="85.5" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:4" ht="90" x14ac:dyDescent="0.2">
       <c r="A41" s="6" t="s">
         <v>79</v>
       </c>
@@ -3551,7 +3556,7 @@
         <v>21880</v>
       </c>
     </row>
-    <row r="42" spans="1:4" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:4" ht="75" x14ac:dyDescent="0.2">
       <c r="A42" s="6" t="s">
         <v>81</v>
       </c>
@@ -3565,7 +3570,7 @@
         <v>22310</v>
       </c>
     </row>
-    <row r="43" spans="1:4" ht="85.5" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:4" ht="90" x14ac:dyDescent="0.2">
       <c r="A43" s="6" t="s">
         <v>83</v>
       </c>
@@ -3579,7 +3584,7 @@
         <v>29298</v>
       </c>
     </row>
-    <row r="44" spans="1:4" ht="99.75" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:4" ht="105" x14ac:dyDescent="0.2">
       <c r="A44" s="6" t="s">
         <v>84</v>
       </c>
@@ -3593,7 +3598,7 @@
         <v>27472</v>
       </c>
     </row>
-    <row r="45" spans="1:4" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:4" ht="75" x14ac:dyDescent="0.2">
       <c r="A45" s="6" t="s">
         <v>86</v>
       </c>
@@ -3607,7 +3612,7 @@
         <v>21785</v>
       </c>
     </row>
-    <row r="46" spans="1:4" ht="57" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:4" ht="60" x14ac:dyDescent="0.2">
       <c r="A46" s="6" t="s">
         <v>88</v>
       </c>
@@ -3621,7 +3626,7 @@
         <v>22726</v>
       </c>
     </row>
-    <row r="47" spans="1:4" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:4" ht="75" x14ac:dyDescent="0.2">
       <c r="A47" s="6" t="s">
         <v>90</v>
       </c>
@@ -3635,7 +3640,7 @@
         <v>27656</v>
       </c>
     </row>
-    <row r="48" spans="1:4" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:4" ht="75" x14ac:dyDescent="0.2">
       <c r="A48" s="6" t="s">
         <v>92</v>
       </c>
@@ -3649,7 +3654,7 @@
         <v>24857</v>
       </c>
     </row>
-    <row r="49" spans="1:4" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:4" ht="75" x14ac:dyDescent="0.2">
       <c r="A49" s="6" t="s">
         <v>94</v>
       </c>
@@ -3663,7 +3668,7 @@
         <v>21033</v>
       </c>
     </row>
-    <row r="50" spans="1:4" ht="85.5" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:4" ht="90" x14ac:dyDescent="0.2">
       <c r="A50" s="6" t="s">
         <v>95</v>
       </c>
@@ -3677,7 +3682,7 @@
         <v>23521</v>
       </c>
     </row>
-    <row r="51" spans="1:4" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:4" ht="75" x14ac:dyDescent="0.2">
       <c r="A51" s="6" t="s">
         <v>97</v>
       </c>
@@ -3691,7 +3696,7 @@
         <v>29569</v>
       </c>
     </row>
-    <row r="52" spans="1:4" ht="85.5" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:4" ht="90" x14ac:dyDescent="0.2">
       <c r="A52" s="6" t="s">
         <v>99</v>
       </c>
@@ -3705,7 +3710,7 @@
         <v>25410</v>
       </c>
     </row>
-    <row r="53" spans="1:4" ht="85.5" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:4" ht="90" x14ac:dyDescent="0.2">
       <c r="A53" s="6" t="s">
         <v>101</v>
       </c>
@@ -3719,7 +3724,7 @@
         <v>23657</v>
       </c>
     </row>
-    <row r="54" spans="1:4" ht="85.5" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:4" ht="90" x14ac:dyDescent="0.2">
       <c r="A54" s="6" t="s">
         <v>102</v>
       </c>
@@ -3733,7 +3738,7 @@
         <v>27105</v>
       </c>
     </row>
-    <row r="55" spans="1:4" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:4" ht="75" x14ac:dyDescent="0.2">
       <c r="A55" s="6" t="s">
         <v>104</v>
       </c>
@@ -3747,7 +3752,7 @@
         <v>28588</v>
       </c>
     </row>
-    <row r="56" spans="1:4" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:4" ht="75" x14ac:dyDescent="0.2">
       <c r="A56" s="6" t="s">
         <v>105</v>
       </c>
@@ -3761,7 +3766,7 @@
         <v>23668</v>
       </c>
     </row>
-    <row r="57" spans="1:4" ht="85.5" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:4" ht="90" x14ac:dyDescent="0.2">
       <c r="A57" s="6" t="s">
         <v>106</v>
       </c>
@@ -3775,7 +3780,7 @@
         <v>23700</v>
       </c>
     </row>
-    <row r="58" spans="1:4" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:4" ht="75" x14ac:dyDescent="0.2">
       <c r="A58" s="6" t="s">
         <v>107</v>
       </c>
@@ -3789,7 +3794,7 @@
         <v>27808</v>
       </c>
     </row>
-    <row r="59" spans="1:4" ht="85.5" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:4" ht="90" x14ac:dyDescent="0.2">
       <c r="A59" s="6" t="s">
         <v>109</v>
       </c>
@@ -3803,7 +3808,7 @@
         <v>27042</v>
       </c>
     </row>
-    <row r="60" spans="1:4" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:4" ht="75" x14ac:dyDescent="0.2">
       <c r="A60" s="6" t="s">
         <v>111</v>
       </c>
@@ -3817,7 +3822,7 @@
         <v>23479</v>
       </c>
     </row>
-    <row r="61" spans="1:4" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:4" ht="75" x14ac:dyDescent="0.2">
       <c r="A61" s="6" t="s">
         <v>112</v>
       </c>
@@ -3831,7 +3836,7 @@
         <v>24555</v>
       </c>
     </row>
-    <row r="62" spans="1:4" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:4" ht="75" x14ac:dyDescent="0.2">
       <c r="A62" s="6" t="s">
         <v>113</v>
       </c>
@@ -3845,7 +3850,7 @@
         <v>28852</v>
       </c>
     </row>
-    <row r="63" spans="1:4" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:4" ht="75" x14ac:dyDescent="0.2">
       <c r="A63" s="6" t="s">
         <v>115</v>
       </c>
@@ -3859,7 +3864,7 @@
         <v>28341</v>
       </c>
     </row>
-    <row r="64" spans="1:4" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:4" ht="75" x14ac:dyDescent="0.2">
       <c r="A64" s="6" t="s">
         <v>117</v>
       </c>
@@ -3873,7 +3878,7 @@
         <v>26927</v>
       </c>
     </row>
-    <row r="65" spans="1:4" ht="85.5" x14ac:dyDescent="0.45">
+    <row r="65" spans="1:4" ht="90" x14ac:dyDescent="0.2">
       <c r="A65" s="6" t="s">
         <v>118</v>
       </c>
@@ -3887,7 +3892,7 @@
         <v>22609</v>
       </c>
     </row>
-    <row r="66" spans="1:4" ht="85.5" x14ac:dyDescent="0.45">
+    <row r="66" spans="1:4" ht="90" x14ac:dyDescent="0.2">
       <c r="A66" s="6" t="s">
         <v>120</v>
       </c>
@@ -3901,7 +3906,7 @@
         <v>27799</v>
       </c>
     </row>
-    <row r="67" spans="1:4" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="67" spans="1:4" ht="75" x14ac:dyDescent="0.2">
       <c r="A67" s="6" t="s">
         <v>122</v>
       </c>
@@ -3915,7 +3920,7 @@
         <v>28480</v>
       </c>
     </row>
-    <row r="68" spans="1:4" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="68" spans="1:4" ht="75" x14ac:dyDescent="0.2">
       <c r="A68" s="6" t="s">
         <v>124</v>
       </c>
@@ -3929,7 +3934,7 @@
         <v>27559</v>
       </c>
     </row>
-    <row r="69" spans="1:4" ht="85.5" x14ac:dyDescent="0.45">
+    <row r="69" spans="1:4" ht="90" x14ac:dyDescent="0.2">
       <c r="A69" s="6" t="s">
         <v>125</v>
       </c>
@@ -3943,7 +3948,7 @@
         <v>27371</v>
       </c>
     </row>
-    <row r="70" spans="1:4" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="70" spans="1:4" ht="75" x14ac:dyDescent="0.2">
       <c r="A70" s="6" t="s">
         <v>127</v>
       </c>
@@ -3957,7 +3962,7 @@
         <v>27178</v>
       </c>
     </row>
-    <row r="71" spans="1:4" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="71" spans="1:4" ht="75" x14ac:dyDescent="0.2">
       <c r="A71" s="6" t="s">
         <v>128</v>
       </c>
@@ -3971,7 +3976,7 @@
         <v>27991</v>
       </c>
     </row>
-    <row r="72" spans="1:4" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="72" spans="1:4" ht="75" x14ac:dyDescent="0.2">
       <c r="A72" s="6" t="s">
         <v>129</v>
       </c>
@@ -3985,7 +3990,7 @@
         <v>29143</v>
       </c>
     </row>
-    <row r="73" spans="1:4" ht="85.5" x14ac:dyDescent="0.45">
+    <row r="73" spans="1:4" ht="90" x14ac:dyDescent="0.2">
       <c r="A73" s="6" t="s">
         <v>131</v>
       </c>
@@ -3999,7 +4004,7 @@
         <v>23811</v>
       </c>
     </row>
-    <row r="74" spans="1:4" ht="85.5" x14ac:dyDescent="0.45">
+    <row r="74" spans="1:4" ht="90" x14ac:dyDescent="0.2">
       <c r="A74" s="6" t="s">
         <v>133</v>
       </c>
@@ -4013,7 +4018,7 @@
         <v>28145</v>
       </c>
     </row>
-    <row r="75" spans="1:4" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="75" spans="1:4" ht="75" x14ac:dyDescent="0.2">
       <c r="A75" s="6" t="s">
         <v>135</v>
       </c>
@@ -4027,7 +4032,7 @@
         <v>23229</v>
       </c>
     </row>
-    <row r="76" spans="1:4" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="76" spans="1:4" ht="75" x14ac:dyDescent="0.2">
       <c r="A76" s="6" t="s">
         <v>137</v>
       </c>
@@ -4041,7 +4046,7 @@
         <v>25236</v>
       </c>
     </row>
-    <row r="77" spans="1:4" ht="85.5" x14ac:dyDescent="0.45">
+    <row r="77" spans="1:4" ht="90" x14ac:dyDescent="0.2">
       <c r="A77" s="6" t="s">
         <v>138</v>
       </c>
@@ -4055,7 +4060,7 @@
         <v>29306</v>
       </c>
     </row>
-    <row r="78" spans="1:4" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="78" spans="1:4" ht="75" x14ac:dyDescent="0.2">
       <c r="A78" s="6" t="s">
         <v>139</v>
       </c>
@@ -4069,7 +4074,7 @@
         <v>23204</v>
       </c>
     </row>
-    <row r="79" spans="1:4" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="79" spans="1:4" ht="75" x14ac:dyDescent="0.2">
       <c r="A79" s="6" t="s">
         <v>140</v>
       </c>
@@ -4083,7 +4088,7 @@
         <v>27284</v>
       </c>
     </row>
-    <row r="80" spans="1:4" ht="85.5" x14ac:dyDescent="0.45">
+    <row r="80" spans="1:4" ht="75" x14ac:dyDescent="0.2">
       <c r="A80" s="6" t="s">
         <v>142</v>
       </c>
@@ -4097,7 +4102,7 @@
         <v>22123</v>
       </c>
     </row>
-    <row r="81" spans="1:4" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="81" spans="1:4" ht="75" x14ac:dyDescent="0.2">
       <c r="A81" s="6" t="s">
         <v>144</v>
       </c>
@@ -4111,7 +4116,7 @@
         <v>21116</v>
       </c>
     </row>
-    <row r="82" spans="1:4" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="82" spans="1:4" ht="75" x14ac:dyDescent="0.2">
       <c r="A82" s="6" t="s">
         <v>146</v>
       </c>
@@ -4125,7 +4130,7 @@
         <v>26985</v>
       </c>
     </row>
-    <row r="83" spans="1:4" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="83" spans="1:4" ht="75" x14ac:dyDescent="0.2">
       <c r="A83" s="6" t="s">
         <v>148</v>
       </c>
@@ -4139,7 +4144,7 @@
         <v>22739</v>
       </c>
     </row>
-    <row r="84" spans="1:4" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="84" spans="1:4" ht="75" x14ac:dyDescent="0.2">
       <c r="A84" s="6" t="s">
         <v>150</v>
       </c>
@@ -4153,7 +4158,7 @@
         <v>29347</v>
       </c>
     </row>
-    <row r="85" spans="1:4" ht="85.5" x14ac:dyDescent="0.45">
+    <row r="85" spans="1:4" ht="90" x14ac:dyDescent="0.2">
       <c r="A85" s="6" t="s">
         <v>152</v>
       </c>
@@ -4167,7 +4172,7 @@
         <v>21269</v>
       </c>
     </row>
-    <row r="86" spans="1:4" ht="85.5" x14ac:dyDescent="0.45">
+    <row r="86" spans="1:4" ht="90" x14ac:dyDescent="0.2">
       <c r="A86" s="6" t="s">
         <v>154</v>
       </c>
@@ -4181,7 +4186,7 @@
         <v>28474</v>
       </c>
     </row>
-    <row r="87" spans="1:4" ht="57" x14ac:dyDescent="0.45">
+    <row r="87" spans="1:4" ht="60" x14ac:dyDescent="0.2">
       <c r="A87" s="6" t="s">
         <v>155</v>
       </c>
@@ -4195,7 +4200,7 @@
         <v>27724</v>
       </c>
     </row>
-    <row r="88" spans="1:4" ht="85.5" x14ac:dyDescent="0.45">
+    <row r="88" spans="1:4" ht="90" x14ac:dyDescent="0.2">
       <c r="A88" s="6" t="s">
         <v>157</v>
       </c>
@@ -4209,7 +4214,7 @@
         <v>22861</v>
       </c>
     </row>
-    <row r="89" spans="1:4" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="89" spans="1:4" ht="75" x14ac:dyDescent="0.2">
       <c r="A89" s="6" t="s">
         <v>158</v>
       </c>
@@ -4223,7 +4228,7 @@
         <v>21017</v>
       </c>
     </row>
-    <row r="90" spans="1:4" ht="57" x14ac:dyDescent="0.45">
+    <row r="90" spans="1:4" ht="60" x14ac:dyDescent="0.2">
       <c r="A90" s="6" t="s">
         <v>160</v>
       </c>
@@ -4237,7 +4242,7 @@
         <v>27852</v>
       </c>
     </row>
-    <row r="91" spans="1:4" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="91" spans="1:4" ht="75" x14ac:dyDescent="0.2">
       <c r="A91" s="6" t="s">
         <v>162</v>
       </c>
@@ -4251,7 +4256,7 @@
         <v>23353</v>
       </c>
     </row>
-    <row r="92" spans="1:4" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="92" spans="1:4" ht="75" x14ac:dyDescent="0.2">
       <c r="A92" s="6" t="s">
         <v>163</v>
       </c>
@@ -4265,7 +4270,7 @@
         <v>21866</v>
       </c>
     </row>
-    <row r="93" spans="1:4" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="93" spans="1:4" ht="75" x14ac:dyDescent="0.2">
       <c r="A93" s="6" t="s">
         <v>164</v>
       </c>
@@ -4279,7 +4284,7 @@
         <v>28397</v>
       </c>
     </row>
-    <row r="94" spans="1:4" ht="85.5" x14ac:dyDescent="0.45">
+    <row r="94" spans="1:4" ht="90" x14ac:dyDescent="0.2">
       <c r="A94" s="6" t="s">
         <v>165</v>
       </c>
@@ -4293,7 +4298,7 @@
         <v>23269</v>
       </c>
     </row>
-    <row r="95" spans="1:4" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="95" spans="1:4" ht="75" x14ac:dyDescent="0.2">
       <c r="A95" s="6" t="s">
         <v>167</v>
       </c>
@@ -4307,7 +4312,7 @@
         <v>24628</v>
       </c>
     </row>
-    <row r="96" spans="1:4" ht="57" x14ac:dyDescent="0.45">
+    <row r="96" spans="1:4" ht="60" x14ac:dyDescent="0.2">
       <c r="A96" s="6" t="s">
         <v>169</v>
       </c>
@@ -4321,7 +4326,7 @@
         <v>22127</v>
       </c>
     </row>
-    <row r="97" spans="1:4" ht="85.5" x14ac:dyDescent="0.45">
+    <row r="97" spans="1:4" ht="90" x14ac:dyDescent="0.2">
       <c r="A97" s="6" t="s">
         <v>171</v>
       </c>
@@ -4335,7 +4340,7 @@
         <v>25136</v>
       </c>
     </row>
-    <row r="98" spans="1:4" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="98" spans="1:4" ht="75" x14ac:dyDescent="0.2">
       <c r="A98" s="6" t="s">
         <v>173</v>
       </c>
@@ -4349,7 +4354,7 @@
         <v>21744</v>
       </c>
     </row>
-    <row r="99" spans="1:4" ht="85.5" x14ac:dyDescent="0.45">
+    <row r="99" spans="1:4" ht="90" x14ac:dyDescent="0.2">
       <c r="A99" s="6" t="s">
         <v>175</v>
       </c>
@@ -4363,7 +4368,7 @@
         <v>29699</v>
       </c>
     </row>
-    <row r="100" spans="1:4" ht="85.5" x14ac:dyDescent="0.45">
+    <row r="100" spans="1:4" ht="90" x14ac:dyDescent="0.2">
       <c r="A100" s="6" t="s">
         <v>177</v>
       </c>
@@ -4377,7 +4382,7 @@
         <v>23887</v>
       </c>
     </row>
-    <row r="101" spans="1:4" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="101" spans="1:4" ht="75" x14ac:dyDescent="0.2">
       <c r="A101" s="6" t="s">
         <v>178</v>
       </c>
@@ -4391,7 +4396,7 @@
         <v>24954</v>
       </c>
     </row>
-    <row r="102" spans="1:4" ht="85.5" x14ac:dyDescent="0.45">
+    <row r="102" spans="1:4" ht="90" x14ac:dyDescent="0.2">
       <c r="A102" s="6" t="s">
         <v>180</v>
       </c>
@@ -4405,7 +4410,7 @@
         <v>25263</v>
       </c>
     </row>
-    <row r="103" spans="1:4" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="103" spans="1:4" ht="75" x14ac:dyDescent="0.2">
       <c r="A103" s="6" t="s">
         <v>182</v>
       </c>
@@ -4419,7 +4424,7 @@
         <v>23713</v>
       </c>
     </row>
-    <row r="104" spans="1:4" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="104" spans="1:4" ht="75" x14ac:dyDescent="0.2">
       <c r="A104" s="6" t="s">
         <v>184</v>
       </c>
@@ -4433,7 +4438,7 @@
         <v>29340</v>
       </c>
     </row>
-    <row r="105" spans="1:4" ht="85.5" x14ac:dyDescent="0.45">
+    <row r="105" spans="1:4" ht="90" x14ac:dyDescent="0.2">
       <c r="A105" s="6" t="s">
         <v>186</v>
       </c>
@@ -4447,7 +4452,7 @@
         <v>26786</v>
       </c>
     </row>
-    <row r="106" spans="1:4" ht="85.5" x14ac:dyDescent="0.45">
+    <row r="106" spans="1:4" ht="90" x14ac:dyDescent="0.2">
       <c r="A106" s="6" t="s">
         <v>188</v>
       </c>
@@ -4461,7 +4466,7 @@
         <v>25756</v>
       </c>
     </row>
-    <row r="107" spans="1:4" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="107" spans="1:4" ht="75" x14ac:dyDescent="0.2">
       <c r="A107" s="6" t="s">
         <v>189</v>
       </c>
@@ -4475,7 +4480,7 @@
         <v>27064</v>
       </c>
     </row>
-    <row r="108" spans="1:4" ht="99.75" x14ac:dyDescent="0.45">
+    <row r="108" spans="1:4" ht="105" x14ac:dyDescent="0.2">
       <c r="A108" s="6" t="s">
         <v>190</v>
       </c>
@@ -4489,7 +4494,7 @@
         <v>29864</v>
       </c>
     </row>
-    <row r="109" spans="1:4" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="109" spans="1:4" ht="75" x14ac:dyDescent="0.2">
       <c r="A109" s="6" t="s">
         <v>192</v>
       </c>
@@ -4503,7 +4508,7 @@
         <v>22078</v>
       </c>
     </row>
-    <row r="110" spans="1:4" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="110" spans="1:4" ht="75" x14ac:dyDescent="0.2">
       <c r="A110" s="6" t="s">
         <v>193</v>
       </c>
@@ -4517,7 +4522,7 @@
         <v>22856</v>
       </c>
     </row>
-    <row r="111" spans="1:4" ht="99.75" x14ac:dyDescent="0.45">
+    <row r="111" spans="1:4" ht="105" x14ac:dyDescent="0.2">
       <c r="A111" s="6" t="s">
         <v>194</v>
       </c>
@@ -4531,7 +4536,7 @@
         <v>24975</v>
       </c>
     </row>
-    <row r="112" spans="1:4" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="112" spans="1:4" ht="75" x14ac:dyDescent="0.2">
       <c r="A112" s="6" t="s">
         <v>196</v>
       </c>
@@ -4545,7 +4550,7 @@
         <v>23914</v>
       </c>
     </row>
-    <row r="113" spans="1:4" ht="85.5" x14ac:dyDescent="0.45">
+    <row r="113" spans="1:4" ht="90" x14ac:dyDescent="0.2">
       <c r="A113" s="6" t="s">
         <v>198</v>
       </c>
@@ -4559,7 +4564,7 @@
         <v>24871</v>
       </c>
     </row>
-    <row r="114" spans="1:4" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="114" spans="1:4" ht="75" x14ac:dyDescent="0.2">
       <c r="A114" s="6" t="s">
         <v>199</v>
       </c>
@@ -4573,7 +4578,7 @@
         <v>27566</v>
       </c>
     </row>
-    <row r="115" spans="1:4" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="115" spans="1:4" ht="75" x14ac:dyDescent="0.2">
       <c r="A115" s="6" t="s">
         <v>200</v>
       </c>
@@ -4587,7 +4592,7 @@
         <v>22430</v>
       </c>
     </row>
-    <row r="116" spans="1:4" ht="99.75" x14ac:dyDescent="0.45">
+    <row r="116" spans="1:4" ht="105" x14ac:dyDescent="0.2">
       <c r="A116" s="6" t="s">
         <v>201</v>
       </c>
@@ -4601,7 +4606,7 @@
         <v>27065</v>
       </c>
     </row>
-    <row r="117" spans="1:4" ht="85.5" x14ac:dyDescent="0.45">
+    <row r="117" spans="1:4" ht="90" x14ac:dyDescent="0.2">
       <c r="A117" s="6" t="s">
         <v>203</v>
       </c>
@@ -4615,7 +4620,7 @@
         <v>27315</v>
       </c>
     </row>
-    <row r="118" spans="1:4" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="118" spans="1:4" ht="75" x14ac:dyDescent="0.2">
       <c r="A118" s="6" t="s">
         <v>205</v>
       </c>
@@ -4629,7 +4634,7 @@
         <v>29426</v>
       </c>
     </row>
-    <row r="119" spans="1:4" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="119" spans="1:4" ht="75" x14ac:dyDescent="0.2">
       <c r="A119" s="6" t="s">
         <v>206</v>
       </c>
@@ -4643,7 +4648,7 @@
         <v>27580</v>
       </c>
     </row>
-    <row r="120" spans="1:4" ht="85.5" x14ac:dyDescent="0.45">
+    <row r="120" spans="1:4" ht="90" x14ac:dyDescent="0.2">
       <c r="A120" s="6" t="s">
         <v>208</v>
       </c>
@@ -4657,7 +4662,7 @@
         <v>26585</v>
       </c>
     </row>
-    <row r="121" spans="1:4" ht="57" x14ac:dyDescent="0.45">
+    <row r="121" spans="1:4" ht="60" x14ac:dyDescent="0.2">
       <c r="A121" s="6" t="s">
         <v>209</v>
       </c>
@@ -4671,7 +4676,7 @@
         <v>22206</v>
       </c>
     </row>
-    <row r="122" spans="1:4" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="122" spans="1:4" ht="75" x14ac:dyDescent="0.2">
       <c r="A122" s="6" t="s">
         <v>210</v>
       </c>
@@ -4685,7 +4690,7 @@
         <v>29932</v>
       </c>
     </row>
-    <row r="123" spans="1:4" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="123" spans="1:4" ht="75" x14ac:dyDescent="0.2">
       <c r="A123" s="6" t="s">
         <v>212</v>
       </c>
@@ -4699,7 +4704,7 @@
         <v>21510</v>
       </c>
     </row>
-    <row r="124" spans="1:4" ht="85.5" x14ac:dyDescent="0.45">
+    <row r="124" spans="1:4" ht="90" x14ac:dyDescent="0.2">
       <c r="A124" s="6" t="s">
         <v>214</v>
       </c>
@@ -4713,7 +4718,7 @@
         <v>26036</v>
       </c>
     </row>
-    <row r="125" spans="1:4" ht="85.5" x14ac:dyDescent="0.45">
+    <row r="125" spans="1:4" ht="90" x14ac:dyDescent="0.2">
       <c r="A125" s="6" t="s">
         <v>216</v>
       </c>
@@ -4727,7 +4732,7 @@
         <v>21303</v>
       </c>
     </row>
-    <row r="126" spans="1:4" ht="57" x14ac:dyDescent="0.45">
+    <row r="126" spans="1:4" ht="60" x14ac:dyDescent="0.2">
       <c r="A126" s="6" t="s">
         <v>218</v>
       </c>
@@ -4741,7 +4746,7 @@
         <v>26366</v>
       </c>
     </row>
-    <row r="127" spans="1:4" ht="57" x14ac:dyDescent="0.45">
+    <row r="127" spans="1:4" ht="60" x14ac:dyDescent="0.2">
       <c r="A127" s="6" t="s">
         <v>219</v>
       </c>
@@ -4755,7 +4760,7 @@
         <v>28884</v>
       </c>
     </row>
-    <row r="128" spans="1:4" ht="85.5" x14ac:dyDescent="0.45">
+    <row r="128" spans="1:4" ht="90" x14ac:dyDescent="0.2">
       <c r="A128" s="6" t="s">
         <v>221</v>
       </c>
@@ -4769,7 +4774,7 @@
         <v>29445</v>
       </c>
     </row>
-    <row r="129" spans="1:4" ht="57" x14ac:dyDescent="0.45">
+    <row r="129" spans="1:4" ht="60" x14ac:dyDescent="0.2">
       <c r="A129" s="6" t="s">
         <v>223</v>
       </c>
@@ -4783,7 +4788,7 @@
         <v>28856</v>
       </c>
     </row>
-    <row r="130" spans="1:4" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="130" spans="1:4" ht="75" x14ac:dyDescent="0.2">
       <c r="A130" s="6" t="s">
         <v>225</v>
       </c>
@@ -4797,7 +4802,7 @@
         <v>23550</v>
       </c>
     </row>
-    <row r="131" spans="1:4" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="131" spans="1:4" ht="75" x14ac:dyDescent="0.2">
       <c r="A131" s="6" t="s">
         <v>226</v>
       </c>
@@ -4811,7 +4816,7 @@
         <v>29639</v>
       </c>
     </row>
-    <row r="132" spans="1:4" ht="85.5" x14ac:dyDescent="0.45">
+    <row r="132" spans="1:4" ht="90" x14ac:dyDescent="0.2">
       <c r="A132" s="6" t="s">
         <v>227</v>
       </c>
@@ -4825,7 +4830,7 @@
         <v>27684</v>
       </c>
     </row>
-    <row r="133" spans="1:4" ht="57" x14ac:dyDescent="0.45">
+    <row r="133" spans="1:4" ht="60" x14ac:dyDescent="0.2">
       <c r="A133" s="6" t="s">
         <v>229</v>
       </c>
@@ -4839,7 +4844,7 @@
         <v>26539</v>
       </c>
     </row>
-    <row r="134" spans="1:4" ht="57" x14ac:dyDescent="0.45">
+    <row r="134" spans="1:4" ht="60" x14ac:dyDescent="0.2">
       <c r="A134" s="6" t="s">
         <v>231</v>
       </c>
@@ -4853,7 +4858,7 @@
         <v>24934</v>
       </c>
     </row>
-    <row r="135" spans="1:4" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="135" spans="1:4" ht="75" x14ac:dyDescent="0.2">
       <c r="A135" s="6" t="s">
         <v>233</v>
       </c>
@@ -4867,7 +4872,7 @@
         <v>25461</v>
       </c>
     </row>
-    <row r="136" spans="1:4" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="136" spans="1:4" ht="75" x14ac:dyDescent="0.2">
       <c r="A136" s="6" t="s">
         <v>235</v>
       </c>
@@ -4881,7 +4886,7 @@
         <v>26951</v>
       </c>
     </row>
-    <row r="137" spans="1:4" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="137" spans="1:4" ht="75" x14ac:dyDescent="0.2">
       <c r="A137" s="6" t="s">
         <v>237</v>
       </c>
@@ -4895,7 +4900,7 @@
         <v>23883</v>
       </c>
     </row>
-    <row r="138" spans="1:4" ht="85.5" x14ac:dyDescent="0.45">
+    <row r="138" spans="1:4" ht="90" x14ac:dyDescent="0.2">
       <c r="A138" s="6" t="s">
         <v>238</v>
       </c>
@@ -4909,7 +4914,7 @@
         <v>29609</v>
       </c>
     </row>
-    <row r="139" spans="1:4" ht="85.5" x14ac:dyDescent="0.45">
+    <row r="139" spans="1:4" ht="90" x14ac:dyDescent="0.2">
       <c r="A139" s="6" t="s">
         <v>240</v>
       </c>
@@ -4923,7 +4928,7 @@
         <v>25217</v>
       </c>
     </row>
-    <row r="140" spans="1:4" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="140" spans="1:4" ht="75" x14ac:dyDescent="0.2">
       <c r="A140" s="6" t="s">
         <v>242</v>
       </c>
@@ -4937,7 +4942,7 @@
         <v>25431</v>
       </c>
     </row>
-    <row r="141" spans="1:4" ht="85.5" x14ac:dyDescent="0.45">
+    <row r="141" spans="1:4" ht="90" x14ac:dyDescent="0.2">
       <c r="A141" s="6" t="s">
         <v>243</v>
       </c>
@@ -4951,7 +4956,7 @@
         <v>28821</v>
       </c>
     </row>
-    <row r="142" spans="1:4" ht="57" x14ac:dyDescent="0.45">
+    <row r="142" spans="1:4" ht="60" x14ac:dyDescent="0.2">
       <c r="A142" s="6" t="s">
         <v>244</v>
       </c>
@@ -4965,7 +4970,7 @@
         <v>24640</v>
       </c>
     </row>
-    <row r="143" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="143" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A143" s="6" t="s">
         <v>246</v>
       </c>
@@ -4979,7 +4984,7 @@
         <v>25961</v>
       </c>
     </row>
-    <row r="144" spans="1:4" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="144" spans="1:4" ht="75" x14ac:dyDescent="0.2">
       <c r="A144" s="6" t="s">
         <v>247</v>
       </c>
@@ -4993,7 +4998,7 @@
         <v>21562</v>
       </c>
     </row>
-    <row r="145" spans="1:4" ht="85.5" x14ac:dyDescent="0.45">
+    <row r="145" spans="1:4" ht="90" x14ac:dyDescent="0.2">
       <c r="A145" s="6" t="s">
         <v>249</v>
       </c>
@@ -5007,7 +5012,7 @@
         <v>26173</v>
       </c>
     </row>
-    <row r="146" spans="1:4" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="146" spans="1:4" ht="75" x14ac:dyDescent="0.2">
       <c r="A146" s="6" t="s">
         <v>250</v>
       </c>
@@ -5021,7 +5026,7 @@
         <v>24809</v>
       </c>
     </row>
-    <row r="147" spans="1:4" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="147" spans="1:4" ht="75" x14ac:dyDescent="0.2">
       <c r="A147" s="6" t="s">
         <v>252</v>
       </c>
@@ -5035,7 +5040,7 @@
         <v>26731</v>
       </c>
     </row>
-    <row r="148" spans="1:4" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="148" spans="1:4" ht="75" x14ac:dyDescent="0.2">
       <c r="A148" s="6" t="s">
         <v>254</v>
       </c>
@@ -5049,7 +5054,7 @@
         <v>22618</v>
       </c>
     </row>
-    <row r="149" spans="1:4" ht="85.5" x14ac:dyDescent="0.45">
+    <row r="149" spans="1:4" ht="90" x14ac:dyDescent="0.2">
       <c r="A149" s="6" t="s">
         <v>256</v>
       </c>
@@ -5063,7 +5068,7 @@
         <v>26081</v>
       </c>
     </row>
-    <row r="150" spans="1:4" ht="85.5" x14ac:dyDescent="0.45">
+    <row r="150" spans="1:4" ht="90" x14ac:dyDescent="0.2">
       <c r="A150" s="6" t="s">
         <v>257</v>
       </c>
@@ -5077,7 +5082,7 @@
         <v>22608</v>
       </c>
     </row>
-    <row r="151" spans="1:4" ht="85.5" x14ac:dyDescent="0.45">
+    <row r="151" spans="1:4" ht="90" x14ac:dyDescent="0.2">
       <c r="A151" s="6" t="s">
         <v>259</v>
       </c>
@@ -5091,7 +5096,7 @@
         <v>21703</v>
       </c>
     </row>
-    <row r="152" spans="1:4" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="152" spans="1:4" ht="75" x14ac:dyDescent="0.2">
       <c r="A152" s="6" t="s">
         <v>260</v>
       </c>
@@ -5105,7 +5110,7 @@
         <v>22254</v>
       </c>
     </row>
-    <row r="153" spans="1:4" ht="85.5" x14ac:dyDescent="0.45">
+    <row r="153" spans="1:4" ht="90" x14ac:dyDescent="0.2">
       <c r="A153" s="6" t="s">
         <v>262</v>
       </c>
@@ -5119,7 +5124,7 @@
         <v>26814</v>
       </c>
     </row>
-    <row r="154" spans="1:4" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="154" spans="1:4" ht="75" x14ac:dyDescent="0.2">
       <c r="A154" s="6" t="s">
         <v>264</v>
       </c>
@@ -5133,7 +5138,7 @@
         <v>27073</v>
       </c>
     </row>
-    <row r="155" spans="1:4" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="155" spans="1:4" ht="75" x14ac:dyDescent="0.2">
       <c r="A155" s="6" t="s">
         <v>265</v>
       </c>
@@ -5147,7 +5152,7 @@
         <v>29203</v>
       </c>
     </row>
-    <row r="156" spans="1:4" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="156" spans="1:4" ht="75" x14ac:dyDescent="0.2">
       <c r="A156" s="6" t="s">
         <v>266</v>
       </c>
@@ -5161,7 +5166,7 @@
         <v>21050</v>
       </c>
     </row>
-    <row r="157" spans="1:4" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="157" spans="1:4" ht="75" x14ac:dyDescent="0.2">
       <c r="A157" s="6" t="s">
         <v>267</v>
       </c>
@@ -5175,7 +5180,7 @@
         <v>21362</v>
       </c>
     </row>
-    <row r="158" spans="1:4" ht="57" x14ac:dyDescent="0.45">
+    <row r="158" spans="1:4" ht="60" x14ac:dyDescent="0.2">
       <c r="A158" s="6" t="s">
         <v>268</v>
       </c>
@@ -5189,7 +5194,7 @@
         <v>22884</v>
       </c>
     </row>
-    <row r="159" spans="1:4" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="159" spans="1:4" ht="75" x14ac:dyDescent="0.2">
       <c r="A159" s="6" t="s">
         <v>270</v>
       </c>
@@ -5203,7 +5208,7 @@
         <v>21828</v>
       </c>
     </row>
-    <row r="160" spans="1:4" ht="85.5" x14ac:dyDescent="0.45">
+    <row r="160" spans="1:4" ht="90" x14ac:dyDescent="0.2">
       <c r="A160" s="6" t="s">
         <v>272</v>
       </c>
@@ -5217,7 +5222,7 @@
         <v>26114</v>
       </c>
     </row>
-    <row r="161" spans="1:4" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="161" spans="1:4" ht="75" x14ac:dyDescent="0.2">
       <c r="A161" s="6" t="s">
         <v>274</v>
       </c>
@@ -5231,7 +5236,7 @@
         <v>26426</v>
       </c>
     </row>
-    <row r="162" spans="1:4" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="162" spans="1:4" ht="75" x14ac:dyDescent="0.2">
       <c r="A162" s="6" t="s">
         <v>276</v>
       </c>
@@ -5245,7 +5250,7 @@
         <v>25671</v>
       </c>
     </row>
-    <row r="163" spans="1:4" ht="85.5" x14ac:dyDescent="0.45">
+    <row r="163" spans="1:4" ht="75" x14ac:dyDescent="0.2">
       <c r="A163" s="6" t="s">
         <v>278</v>
       </c>
@@ -5259,7 +5264,7 @@
         <v>26515</v>
       </c>
     </row>
-    <row r="164" spans="1:4" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="164" spans="1:4" ht="75" x14ac:dyDescent="0.2">
       <c r="A164" s="6" t="s">
         <v>280</v>
       </c>
@@ -5273,7 +5278,7 @@
         <v>25965</v>
       </c>
     </row>
-    <row r="165" spans="1:4" ht="85.5" x14ac:dyDescent="0.45">
+    <row r="165" spans="1:4" ht="90" x14ac:dyDescent="0.2">
       <c r="A165" s="6" t="s">
         <v>282</v>
       </c>
@@ -5287,7 +5292,7 @@
         <v>22498</v>
       </c>
     </row>
-    <row r="166" spans="1:4" ht="85.5" x14ac:dyDescent="0.45">
+    <row r="166" spans="1:4" ht="90" x14ac:dyDescent="0.2">
       <c r="A166" s="6" t="s">
         <v>284</v>
       </c>
@@ -5301,7 +5306,7 @@
         <v>29649</v>
       </c>
     </row>
-    <row r="167" spans="1:4" ht="99.75" x14ac:dyDescent="0.45">
+    <row r="167" spans="1:4" ht="105" x14ac:dyDescent="0.2">
       <c r="A167" s="6" t="s">
         <v>582</v>
       </c>
@@ -5315,7 +5320,7 @@
         <v>21344</v>
       </c>
     </row>
-    <row r="168" spans="1:4" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="168" spans="1:4" ht="75" x14ac:dyDescent="0.2">
       <c r="A168" s="6" t="s">
         <v>286</v>
       </c>
@@ -5329,7 +5334,7 @@
         <v>29035</v>
       </c>
     </row>
-    <row r="169" spans="1:4" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="169" spans="1:4" ht="75" x14ac:dyDescent="0.2">
       <c r="A169" s="6" t="s">
         <v>288</v>
       </c>
@@ -5343,7 +5348,7 @@
         <v>25239</v>
       </c>
     </row>
-    <row r="170" spans="1:4" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="170" spans="1:4" ht="75" x14ac:dyDescent="0.2">
       <c r="A170" s="6" t="s">
         <v>290</v>
       </c>
@@ -5357,7 +5362,7 @@
         <v>24364</v>
       </c>
     </row>
-    <row r="171" spans="1:4" ht="57" x14ac:dyDescent="0.45">
+    <row r="171" spans="1:4" ht="60" x14ac:dyDescent="0.2">
       <c r="A171" s="6" t="s">
         <v>292</v>
       </c>
@@ -5371,7 +5376,7 @@
         <v>29250</v>
       </c>
     </row>
-    <row r="172" spans="1:4" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="172" spans="1:4" ht="75" x14ac:dyDescent="0.2">
       <c r="A172" s="6" t="s">
         <v>294</v>
       </c>
@@ -5385,7 +5390,7 @@
         <v>23439</v>
       </c>
     </row>
-    <row r="173" spans="1:4" ht="85.5" x14ac:dyDescent="0.45">
+    <row r="173" spans="1:4" ht="90" x14ac:dyDescent="0.2">
       <c r="A173" s="6" t="s">
         <v>296</v>
       </c>
@@ -5399,7 +5404,7 @@
         <v>25323</v>
       </c>
     </row>
-    <row r="174" spans="1:4" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="174" spans="1:4" ht="75" x14ac:dyDescent="0.2">
       <c r="A174" s="6" t="s">
         <v>297</v>
       </c>
@@ -5413,7 +5418,7 @@
         <v>26610</v>
       </c>
     </row>
-    <row r="175" spans="1:4" ht="57" x14ac:dyDescent="0.45">
+    <row r="175" spans="1:4" ht="60" x14ac:dyDescent="0.2">
       <c r="A175" s="6" t="s">
         <v>298</v>
       </c>
@@ -5427,7 +5432,7 @@
         <v>24955</v>
       </c>
     </row>
-    <row r="176" spans="1:4" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="176" spans="1:4" ht="60" x14ac:dyDescent="0.2">
       <c r="A176" s="6" t="s">
         <v>300</v>
       </c>
@@ -5441,7 +5446,7 @@
         <v>22488</v>
       </c>
     </row>
-    <row r="177" spans="1:4" ht="57" x14ac:dyDescent="0.45">
+    <row r="177" spans="1:4" ht="60" x14ac:dyDescent="0.2">
       <c r="A177" s="6" t="s">
         <v>302</v>
       </c>
@@ -5455,7 +5460,7 @@
         <v>26633</v>
       </c>
     </row>
-    <row r="178" spans="1:4" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="178" spans="1:4" ht="75" x14ac:dyDescent="0.2">
       <c r="A178" s="6" t="s">
         <v>304</v>
       </c>
@@ -5469,7 +5474,7 @@
         <v>22455</v>
       </c>
     </row>
-    <row r="179" spans="1:4" ht="85.5" x14ac:dyDescent="0.45">
+    <row r="179" spans="1:4" ht="90" x14ac:dyDescent="0.2">
       <c r="A179" s="6" t="s">
         <v>305</v>
       </c>
@@ -5483,7 +5488,7 @@
         <v>28885</v>
       </c>
     </row>
-    <row r="180" spans="1:4" ht="57" x14ac:dyDescent="0.45">
+    <row r="180" spans="1:4" ht="60" x14ac:dyDescent="0.2">
       <c r="A180" s="6" t="s">
         <v>307</v>
       </c>
@@ -5497,7 +5502,7 @@
         <v>24820</v>
       </c>
     </row>
-    <row r="181" spans="1:4" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="181" spans="1:4" ht="75" x14ac:dyDescent="0.2">
       <c r="A181" s="6" t="s">
         <v>309</v>
       </c>
@@ -5511,7 +5516,7 @@
         <v>22148</v>
       </c>
     </row>
-    <row r="182" spans="1:4" ht="85.5" x14ac:dyDescent="0.45">
+    <row r="182" spans="1:4" ht="90" x14ac:dyDescent="0.2">
       <c r="A182" s="6" t="s">
         <v>311</v>
       </c>
@@ -5525,7 +5530,7 @@
         <v>25177</v>
       </c>
     </row>
-    <row r="183" spans="1:4" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="183" spans="1:4" ht="75" x14ac:dyDescent="0.2">
       <c r="A183" s="6" t="s">
         <v>313</v>
       </c>
@@ -5539,7 +5544,7 @@
         <v>26312</v>
       </c>
     </row>
-    <row r="184" spans="1:4" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="184" spans="1:4" ht="75" x14ac:dyDescent="0.2">
       <c r="A184" s="6" t="s">
         <v>315</v>
       </c>
@@ -5553,7 +5558,7 @@
         <v>25899</v>
       </c>
     </row>
-    <row r="185" spans="1:4" ht="85.5" x14ac:dyDescent="0.45">
+    <row r="185" spans="1:4" ht="75" x14ac:dyDescent="0.2">
       <c r="A185" s="6" t="s">
         <v>316</v>
       </c>
@@ -5567,7 +5572,7 @@
         <v>27099</v>
       </c>
     </row>
-    <row r="186" spans="1:4" ht="57" x14ac:dyDescent="0.45">
+    <row r="186" spans="1:4" ht="60" x14ac:dyDescent="0.2">
       <c r="A186" s="6" t="s">
         <v>318</v>
       </c>
@@ -5581,7 +5586,7 @@
         <v>24058</v>
       </c>
     </row>
-    <row r="187" spans="1:4" ht="85.5" x14ac:dyDescent="0.45">
+    <row r="187" spans="1:4" ht="90" x14ac:dyDescent="0.2">
       <c r="A187" s="6" t="s">
         <v>320</v>
       </c>
@@ -5595,7 +5600,7 @@
         <v>21739</v>
       </c>
     </row>
-    <row r="188" spans="1:4" ht="57" x14ac:dyDescent="0.45">
+    <row r="188" spans="1:4" ht="60" x14ac:dyDescent="0.2">
       <c r="A188" s="6" t="s">
         <v>321</v>
       </c>
@@ -5609,7 +5614,7 @@
         <v>28698</v>
       </c>
     </row>
-    <row r="189" spans="1:4" ht="85.5" x14ac:dyDescent="0.45">
+    <row r="189" spans="1:4" ht="90" x14ac:dyDescent="0.2">
       <c r="A189" s="6" t="s">
         <v>323</v>
       </c>
@@ -5623,7 +5628,7 @@
         <v>25292</v>
       </c>
     </row>
-    <row r="190" spans="1:4" ht="85.5" x14ac:dyDescent="0.45">
+    <row r="190" spans="1:4" ht="90" x14ac:dyDescent="0.2">
       <c r="A190" s="6" t="s">
         <v>325</v>
       </c>
@@ -5637,7 +5642,7 @@
         <v>24042</v>
       </c>
     </row>
-    <row r="191" spans="1:4" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="191" spans="1:4" ht="75" x14ac:dyDescent="0.2">
       <c r="A191" s="6" t="s">
         <v>327</v>
       </c>
@@ -5651,7 +5656,7 @@
         <v>27944</v>
       </c>
     </row>
-    <row r="192" spans="1:4" ht="57" x14ac:dyDescent="0.45">
+    <row r="192" spans="1:4" ht="60" x14ac:dyDescent="0.2">
       <c r="A192" s="6" t="s">
         <v>328</v>
       </c>
@@ -5665,7 +5670,7 @@
         <v>25514</v>
       </c>
     </row>
-    <row r="193" spans="1:4" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="193" spans="1:4" ht="75" x14ac:dyDescent="0.2">
       <c r="A193" s="6" t="s">
         <v>329</v>
       </c>
@@ -5679,7 +5684,7 @@
         <v>26391</v>
       </c>
     </row>
-    <row r="194" spans="1:4" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="194" spans="1:4" ht="75" x14ac:dyDescent="0.2">
       <c r="A194" s="6" t="s">
         <v>330</v>
       </c>
@@ -5693,7 +5698,7 @@
         <v>28173</v>
       </c>
     </row>
-    <row r="195" spans="1:4" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="195" spans="1:4" ht="75" x14ac:dyDescent="0.2">
       <c r="A195" s="6" t="s">
         <v>331</v>
       </c>
@@ -5707,7 +5712,7 @@
         <v>25548</v>
       </c>
     </row>
-    <row r="196" spans="1:4" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="196" spans="1:4" ht="75" x14ac:dyDescent="0.2">
       <c r="A196" s="6" t="s">
         <v>333</v>
       </c>
@@ -5721,7 +5726,7 @@
         <v>28422</v>
       </c>
     </row>
-    <row r="197" spans="1:4" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="197" spans="1:4" ht="75" x14ac:dyDescent="0.2">
       <c r="A197" s="6" t="s">
         <v>334</v>
       </c>
@@ -5735,7 +5740,7 @@
         <v>26724</v>
       </c>
     </row>
-    <row r="198" spans="1:4" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="198" spans="1:4" ht="75" x14ac:dyDescent="0.2">
       <c r="A198" s="6" t="s">
         <v>336</v>
       </c>
@@ -5749,7 +5754,7 @@
         <v>25028</v>
       </c>
     </row>
-    <row r="199" spans="1:4" ht="85.5" x14ac:dyDescent="0.45">
+    <row r="199" spans="1:4" ht="75" x14ac:dyDescent="0.2">
       <c r="A199" s="6" t="s">
         <v>338</v>
       </c>
@@ -5763,7 +5768,7 @@
         <v>28119</v>
       </c>
     </row>
-    <row r="200" spans="1:4" ht="57" x14ac:dyDescent="0.45">
+    <row r="200" spans="1:4" ht="60" x14ac:dyDescent="0.2">
       <c r="A200" s="6" t="s">
         <v>339</v>
       </c>
@@ -5777,7 +5782,7 @@
         <v>28870</v>
       </c>
     </row>
-    <row r="201" spans="1:4" ht="85.5" x14ac:dyDescent="0.45">
+    <row r="201" spans="1:4" ht="90" x14ac:dyDescent="0.2">
       <c r="A201" s="6" t="s">
         <v>341</v>
       </c>
@@ -5791,7 +5796,7 @@
         <v>27297</v>
       </c>
     </row>
-    <row r="202" spans="1:4" ht="85.5" x14ac:dyDescent="0.45">
+    <row r="202" spans="1:4" ht="90" x14ac:dyDescent="0.2">
       <c r="A202" s="6" t="s">
         <v>342</v>
       </c>
@@ -5805,7 +5810,7 @@
         <v>29312</v>
       </c>
     </row>
-    <row r="203" spans="1:4" ht="85.5" x14ac:dyDescent="0.45">
+    <row r="203" spans="1:4" ht="75" x14ac:dyDescent="0.2">
       <c r="A203" s="6" t="s">
         <v>344</v>
       </c>
@@ -5819,7 +5824,7 @@
         <v>25535</v>
       </c>
     </row>
-    <row r="204" spans="1:4" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="204" spans="1:4" ht="75" x14ac:dyDescent="0.2">
       <c r="A204" s="6" t="s">
         <v>346</v>
       </c>
@@ -5833,7 +5838,7 @@
         <v>21880</v>
       </c>
     </row>
-    <row r="205" spans="1:4" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="205" spans="1:4" ht="75" x14ac:dyDescent="0.2">
       <c r="A205" s="6" t="s">
         <v>347</v>
       </c>
@@ -5847,7 +5852,7 @@
         <v>22310</v>
       </c>
     </row>
-    <row r="206" spans="1:4" ht="85.5" x14ac:dyDescent="0.45">
+    <row r="206" spans="1:4" ht="90" x14ac:dyDescent="0.2">
       <c r="A206" s="6" t="s">
         <v>348</v>
       </c>
@@ -5861,7 +5866,7 @@
         <v>29298</v>
       </c>
     </row>
-    <row r="207" spans="1:4" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="207" spans="1:4" ht="75" x14ac:dyDescent="0.2">
       <c r="A207" s="6" t="s">
         <v>349</v>
       </c>
@@ -5875,7 +5880,7 @@
         <v>27472</v>
       </c>
     </row>
-    <row r="208" spans="1:4" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="208" spans="1:4" ht="75" x14ac:dyDescent="0.2">
       <c r="A208" s="6" t="s">
         <v>350</v>
       </c>
@@ -5889,7 +5894,7 @@
         <v>21785</v>
       </c>
     </row>
-    <row r="209" spans="1:4" ht="85.5" x14ac:dyDescent="0.45">
+    <row r="209" spans="1:4" ht="90" x14ac:dyDescent="0.2">
       <c r="A209" s="6" t="s">
         <v>352</v>
       </c>
@@ -5903,7 +5908,7 @@
         <v>22726</v>
       </c>
     </row>
-    <row r="210" spans="1:4" ht="85.5" x14ac:dyDescent="0.45">
+    <row r="210" spans="1:4" ht="90" x14ac:dyDescent="0.2">
       <c r="A210" s="6" t="s">
         <v>354</v>
       </c>
@@ -5917,7 +5922,7 @@
         <v>27656</v>
       </c>
     </row>
-    <row r="211" spans="1:4" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="211" spans="1:4" ht="75" x14ac:dyDescent="0.2">
       <c r="A211" s="6" t="s">
         <v>355</v>
       </c>
@@ -5931,7 +5936,7 @@
         <v>24857</v>
       </c>
     </row>
-    <row r="212" spans="1:4" ht="85.5" x14ac:dyDescent="0.45">
+    <row r="212" spans="1:4" ht="90" x14ac:dyDescent="0.2">
       <c r="A212" s="6" t="s">
         <v>583</v>
       </c>
@@ -5945,7 +5950,7 @@
         <v>21033</v>
       </c>
     </row>
-    <row r="213" spans="1:4" ht="85.5" x14ac:dyDescent="0.45">
+    <row r="213" spans="1:4" ht="75" x14ac:dyDescent="0.2">
       <c r="A213" s="6" t="s">
         <v>357</v>
       </c>
@@ -5959,7 +5964,7 @@
         <v>23521</v>
       </c>
     </row>
-    <row r="214" spans="1:4" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="214" spans="1:4" ht="75" x14ac:dyDescent="0.2">
       <c r="A214" s="6" t="s">
         <v>359</v>
       </c>
@@ -5973,7 +5978,7 @@
         <v>29569</v>
       </c>
     </row>
-    <row r="215" spans="1:4" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="215" spans="1:4" ht="75" x14ac:dyDescent="0.2">
       <c r="A215" s="6" t="s">
         <v>361</v>
       </c>
@@ -5987,7 +5992,7 @@
         <v>25410</v>
       </c>
     </row>
-    <row r="216" spans="1:4" ht="99.75" x14ac:dyDescent="0.45">
+    <row r="216" spans="1:4" ht="105" x14ac:dyDescent="0.2">
       <c r="A216" s="6" t="s">
         <v>362</v>
       </c>
@@ -6001,7 +6006,7 @@
         <v>23657</v>
       </c>
     </row>
-    <row r="217" spans="1:4" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="217" spans="1:4" ht="75" x14ac:dyDescent="0.2">
       <c r="A217" s="6" t="s">
         <v>363</v>
       </c>
@@ -6015,7 +6020,7 @@
         <v>27105</v>
       </c>
     </row>
-    <row r="218" spans="1:4" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="218" spans="1:4" ht="75" x14ac:dyDescent="0.2">
       <c r="A218" s="6" t="s">
         <v>364</v>
       </c>
@@ -6029,7 +6034,7 @@
         <v>28588</v>
       </c>
     </row>
-    <row r="219" spans="1:4" ht="57" x14ac:dyDescent="0.45">
+    <row r="219" spans="1:4" ht="60" x14ac:dyDescent="0.2">
       <c r="A219" s="6" t="s">
         <v>365</v>
       </c>
@@ -6043,7 +6048,7 @@
         <v>23668</v>
       </c>
     </row>
-    <row r="220" spans="1:4" ht="57" x14ac:dyDescent="0.45">
+    <row r="220" spans="1:4" ht="60" x14ac:dyDescent="0.2">
       <c r="A220" s="6" t="s">
         <v>367</v>
       </c>
@@ -6057,7 +6062,7 @@
         <v>23700</v>
       </c>
     </row>
-    <row r="221" spans="1:4" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="221" spans="1:4" ht="75" x14ac:dyDescent="0.2">
       <c r="A221" s="6" t="s">
         <v>369</v>
       </c>
@@ -6071,7 +6076,7 @@
         <v>27808</v>
       </c>
     </row>
-    <row r="222" spans="1:4" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="222" spans="1:4" ht="75" x14ac:dyDescent="0.2">
       <c r="A222" s="6" t="s">
         <v>371</v>
       </c>
@@ -6085,7 +6090,7 @@
         <v>27042</v>
       </c>
     </row>
-    <row r="223" spans="1:4" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="223" spans="1:4" ht="75" x14ac:dyDescent="0.2">
       <c r="A223" s="6" t="s">
         <v>372</v>
       </c>
@@ -6099,7 +6104,7 @@
         <v>23479</v>
       </c>
     </row>
-    <row r="224" spans="1:4" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="224" spans="1:4" ht="75" x14ac:dyDescent="0.2">
       <c r="A224" s="6" t="s">
         <v>374</v>
       </c>
@@ -6113,7 +6118,7 @@
         <v>24555</v>
       </c>
     </row>
-    <row r="225" spans="1:4" ht="85.5" x14ac:dyDescent="0.45">
+    <row r="225" spans="1:4" ht="90" x14ac:dyDescent="0.2">
       <c r="A225" s="11" t="s">
         <v>375</v>
       </c>
@@ -6127,7 +6132,7 @@
         <v>28852</v>
       </c>
     </row>
-    <row r="226" spans="1:4" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="226" spans="1:4" ht="75" x14ac:dyDescent="0.2">
       <c r="A226" s="11" t="s">
         <v>376</v>
       </c>
@@ -6141,7 +6146,7 @@
         <v>28341</v>
       </c>
     </row>
-    <row r="227" spans="1:4" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="227" spans="1:4" ht="75" x14ac:dyDescent="0.2">
       <c r="A227" s="11" t="s">
         <v>377</v>
       </c>
@@ -6155,7 +6160,7 @@
         <v>26927</v>
       </c>
     </row>
-    <row r="228" spans="1:4" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="228" spans="1:4" ht="75" x14ac:dyDescent="0.2">
       <c r="A228" s="11" t="s">
         <v>378</v>
       </c>
@@ -6169,7 +6174,7 @@
         <v>22609</v>
       </c>
     </row>
-    <row r="229" spans="1:4" ht="57" x14ac:dyDescent="0.45">
+    <row r="229" spans="1:4" ht="60" x14ac:dyDescent="0.2">
       <c r="A229" s="11" t="s">
         <v>380</v>
       </c>
@@ -6183,7 +6188,7 @@
         <v>27799</v>
       </c>
     </row>
-    <row r="230" spans="1:4" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="230" spans="1:4" ht="75" x14ac:dyDescent="0.2">
       <c r="A230" s="11" t="s">
         <v>382</v>
       </c>
@@ -6197,7 +6202,7 @@
         <v>28480</v>
       </c>
     </row>
-    <row r="231" spans="1:4" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="231" spans="1:4" ht="75" x14ac:dyDescent="0.2">
       <c r="A231" s="11" t="s">
         <v>384</v>
       </c>
@@ -6211,7 +6216,7 @@
         <v>27559</v>
       </c>
     </row>
-    <row r="232" spans="1:4" ht="57" x14ac:dyDescent="0.45">
+    <row r="232" spans="1:4" ht="60" x14ac:dyDescent="0.2">
       <c r="A232" s="11" t="s">
         <v>385</v>
       </c>
@@ -6225,7 +6230,7 @@
         <v>27371</v>
       </c>
     </row>
-    <row r="233" spans="1:4" ht="85.5" x14ac:dyDescent="0.45">
+    <row r="233" spans="1:4" ht="90" x14ac:dyDescent="0.2">
       <c r="A233" s="11" t="s">
         <v>387</v>
       </c>
@@ -6239,7 +6244,7 @@
         <v>27178</v>
       </c>
     </row>
-    <row r="234" spans="1:4" ht="57" x14ac:dyDescent="0.45">
+    <row r="234" spans="1:4" ht="60" x14ac:dyDescent="0.2">
       <c r="A234" s="11" t="s">
         <v>388</v>
       </c>
@@ -6253,7 +6258,7 @@
         <v>27991</v>
       </c>
     </row>
-    <row r="235" spans="1:4" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="235" spans="1:4" ht="75" x14ac:dyDescent="0.2">
       <c r="A235" s="11" t="s">
         <v>390</v>
       </c>
@@ -6267,7 +6272,7 @@
         <v>29143</v>
       </c>
     </row>
-    <row r="236" spans="1:4" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="236" spans="1:4" ht="75" x14ac:dyDescent="0.2">
       <c r="A236" s="11" t="s">
         <v>391</v>
       </c>
@@ -6281,7 +6286,7 @@
         <v>23811</v>
       </c>
     </row>
-    <row r="237" spans="1:4" ht="57" x14ac:dyDescent="0.45">
+    <row r="237" spans="1:4" ht="60" x14ac:dyDescent="0.2">
       <c r="A237" s="11" t="s">
         <v>392</v>
       </c>
@@ -6295,7 +6300,7 @@
         <v>28145</v>
       </c>
     </row>
-    <row r="238" spans="1:4" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="238" spans="1:4" ht="75" x14ac:dyDescent="0.2">
       <c r="A238" s="11" t="s">
         <v>393</v>
       </c>
@@ -6309,7 +6314,7 @@
         <v>23229</v>
       </c>
     </row>
-    <row r="239" spans="1:4" ht="57" x14ac:dyDescent="0.45">
+    <row r="239" spans="1:4" ht="60" x14ac:dyDescent="0.2">
       <c r="A239" s="11" t="s">
         <v>394</v>
       </c>
@@ -6323,7 +6328,7 @@
         <v>25236</v>
       </c>
     </row>
-    <row r="240" spans="1:4" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="240" spans="1:4" ht="75" x14ac:dyDescent="0.2">
       <c r="A240" s="11" t="s">
         <v>396</v>
       </c>
@@ -6337,7 +6342,7 @@
         <v>29306</v>
       </c>
     </row>
-    <row r="241" spans="1:4" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="241" spans="1:4" ht="75" x14ac:dyDescent="0.2">
       <c r="A241" s="11" t="s">
         <v>398</v>
       </c>
@@ -6351,7 +6356,7 @@
         <v>23204</v>
       </c>
     </row>
-    <row r="242" spans="1:4" ht="57" x14ac:dyDescent="0.45">
+    <row r="242" spans="1:4" ht="60" x14ac:dyDescent="0.2">
       <c r="A242" s="11" t="s">
         <v>399</v>
       </c>
@@ -6365,7 +6370,7 @@
         <v>27284</v>
       </c>
     </row>
-    <row r="243" spans="1:4" ht="85.5" x14ac:dyDescent="0.45">
+    <row r="243" spans="1:4" ht="90" x14ac:dyDescent="0.2">
       <c r="A243" s="11" t="s">
         <v>401</v>
       </c>
@@ -6379,7 +6384,7 @@
         <v>22123</v>
       </c>
     </row>
-    <row r="244" spans="1:4" ht="57" x14ac:dyDescent="0.45">
+    <row r="244" spans="1:4" ht="60" x14ac:dyDescent="0.2">
       <c r="A244" s="11" t="s">
         <v>402</v>
       </c>
@@ -6393,7 +6398,7 @@
         <v>21116</v>
       </c>
     </row>
-    <row r="245" spans="1:4" ht="57" x14ac:dyDescent="0.45">
+    <row r="245" spans="1:4" ht="60" x14ac:dyDescent="0.2">
       <c r="A245" s="11" t="s">
         <v>404</v>
       </c>
@@ -6407,7 +6412,7 @@
         <v>26985</v>
       </c>
     </row>
-    <row r="246" spans="1:4" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="246" spans="1:4" ht="60" x14ac:dyDescent="0.2">
       <c r="A246" s="11" t="s">
         <v>406</v>
       </c>
@@ -6421,7 +6426,7 @@
         <v>22739</v>
       </c>
     </row>
-    <row r="247" spans="1:4" ht="57" x14ac:dyDescent="0.45">
+    <row r="247" spans="1:4" ht="60" x14ac:dyDescent="0.2">
       <c r="A247" s="11" t="s">
         <v>408</v>
       </c>
@@ -6435,7 +6440,7 @@
         <v>29347</v>
       </c>
     </row>
-    <row r="248" spans="1:4" ht="57" x14ac:dyDescent="0.45">
+    <row r="248" spans="1:4" ht="60" x14ac:dyDescent="0.2">
       <c r="A248" s="11" t="s">
         <v>410</v>
       </c>
@@ -6449,7 +6454,7 @@
         <v>21269</v>
       </c>
     </row>
-    <row r="249" spans="1:4" ht="57" x14ac:dyDescent="0.45">
+    <row r="249" spans="1:4" ht="60" x14ac:dyDescent="0.2">
       <c r="A249" s="11" t="s">
         <v>412</v>
       </c>
@@ -6463,7 +6468,7 @@
         <v>28474</v>
       </c>
     </row>
-    <row r="250" spans="1:4" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="250" spans="1:4" ht="75" x14ac:dyDescent="0.2">
       <c r="A250" s="11" t="s">
         <v>414</v>
       </c>
@@ -6477,7 +6482,7 @@
         <v>27724</v>
       </c>
     </row>
-    <row r="251" spans="1:4" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="251" spans="1:4" ht="75" x14ac:dyDescent="0.2">
       <c r="A251" s="11" t="s">
         <v>416</v>
       </c>
@@ -6491,7 +6496,7 @@
         <v>22861</v>
       </c>
     </row>
-    <row r="252" spans="1:4" ht="57" x14ac:dyDescent="0.45">
+    <row r="252" spans="1:4" ht="60" x14ac:dyDescent="0.2">
       <c r="A252" s="11" t="s">
         <v>417</v>
       </c>
@@ -6505,7 +6510,7 @@
         <v>21017</v>
       </c>
     </row>
-    <row r="253" spans="1:4" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="253" spans="1:4" ht="75" x14ac:dyDescent="0.2">
       <c r="A253" s="11" t="s">
         <v>419</v>
       </c>
@@ -6519,7 +6524,7 @@
         <v>27852</v>
       </c>
     </row>
-    <row r="254" spans="1:4" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="254" spans="1:4" ht="75" x14ac:dyDescent="0.2">
       <c r="A254" s="11" t="s">
         <v>421</v>
       </c>
@@ -6533,7 +6538,7 @@
         <v>23353</v>
       </c>
     </row>
-    <row r="255" spans="1:4" ht="85.5" x14ac:dyDescent="0.45">
+    <row r="255" spans="1:4" ht="90" x14ac:dyDescent="0.2">
       <c r="A255" s="11" t="s">
         <v>422</v>
       </c>
@@ -6547,7 +6552,7 @@
         <v>21866</v>
       </c>
     </row>
-    <row r="256" spans="1:4" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="256" spans="1:4" ht="75" x14ac:dyDescent="0.2">
       <c r="A256" s="11" t="s">
         <v>423</v>
       </c>
@@ -6561,7 +6566,7 @@
         <v>28397</v>
       </c>
     </row>
-    <row r="257" spans="1:4" ht="85.5" x14ac:dyDescent="0.45">
+    <row r="257" spans="1:4" ht="90" x14ac:dyDescent="0.2">
       <c r="A257" s="11" t="s">
         <v>424</v>
       </c>
@@ -6575,7 +6580,7 @@
         <v>23269</v>
       </c>
     </row>
-    <row r="258" spans="1:4" ht="57" x14ac:dyDescent="0.45">
+    <row r="258" spans="1:4" ht="60" x14ac:dyDescent="0.2">
       <c r="A258" s="11" t="s">
         <v>425</v>
       </c>
@@ -6589,7 +6594,7 @@
         <v>24628</v>
       </c>
     </row>
-    <row r="259" spans="1:4" ht="57" x14ac:dyDescent="0.45">
+    <row r="259" spans="1:4" ht="60" x14ac:dyDescent="0.2">
       <c r="A259" s="11" t="s">
         <v>427</v>
       </c>
@@ -6603,7 +6608,7 @@
         <v>22127</v>
       </c>
     </row>
-    <row r="260" spans="1:4" ht="57" x14ac:dyDescent="0.45">
+    <row r="260" spans="1:4" ht="60" x14ac:dyDescent="0.2">
       <c r="A260" s="11" t="s">
         <v>429</v>
       </c>
@@ -6617,7 +6622,7 @@
         <v>25136</v>
       </c>
     </row>
-    <row r="261" spans="1:4" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="261" spans="1:4" ht="75" x14ac:dyDescent="0.2">
       <c r="A261" s="11" t="s">
         <v>431</v>
       </c>
@@ -6631,7 +6636,7 @@
         <v>21744</v>
       </c>
     </row>
-    <row r="262" spans="1:4" ht="85.5" x14ac:dyDescent="0.45">
+    <row r="262" spans="1:4" ht="90" x14ac:dyDescent="0.2">
       <c r="A262" s="11" t="s">
         <v>432</v>
       </c>
@@ -6645,7 +6650,7 @@
         <v>29699</v>
       </c>
     </row>
-    <row r="263" spans="1:4" ht="57" x14ac:dyDescent="0.45">
+    <row r="263" spans="1:4" ht="60" x14ac:dyDescent="0.2">
       <c r="A263" s="11" t="s">
         <v>433</v>
       </c>
@@ -6659,7 +6664,7 @@
         <v>23887</v>
       </c>
     </row>
-    <row r="264" spans="1:4" ht="85.5" x14ac:dyDescent="0.45">
+    <row r="264" spans="1:4" ht="90" x14ac:dyDescent="0.2">
       <c r="A264" s="11" t="s">
         <v>435</v>
       </c>
@@ -6673,7 +6678,7 @@
         <v>24954</v>
       </c>
     </row>
-    <row r="265" spans="1:4" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="265" spans="1:4" ht="75" x14ac:dyDescent="0.2">
       <c r="A265" s="11" t="s">
         <v>436</v>
       </c>
@@ -6687,7 +6692,7 @@
         <v>25263</v>
       </c>
     </row>
-    <row r="266" spans="1:4" ht="57" x14ac:dyDescent="0.45">
+    <row r="266" spans="1:4" ht="60" x14ac:dyDescent="0.2">
       <c r="A266" s="11" t="s">
         <v>438</v>
       </c>
@@ -6701,7 +6706,7 @@
         <v>23713</v>
       </c>
     </row>
-    <row r="267" spans="1:4" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="267" spans="1:4" ht="75" x14ac:dyDescent="0.2">
       <c r="A267" s="11" t="s">
         <v>440</v>
       </c>
@@ -6715,7 +6720,7 @@
         <v>29340</v>
       </c>
     </row>
-    <row r="268" spans="1:4" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="268" spans="1:4" ht="75" x14ac:dyDescent="0.2">
       <c r="A268" s="11" t="s">
         <v>442</v>
       </c>
@@ -6729,7 +6734,7 @@
         <v>26786</v>
       </c>
     </row>
-    <row r="269" spans="1:4" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="269" spans="1:4" ht="75" x14ac:dyDescent="0.2">
       <c r="A269" s="11" t="s">
         <v>443</v>
       </c>
@@ -6743,7 +6748,7 @@
         <v>25756</v>
       </c>
     </row>
-    <row r="270" spans="1:4" ht="57" x14ac:dyDescent="0.45">
+    <row r="270" spans="1:4" ht="60" x14ac:dyDescent="0.2">
       <c r="A270" s="11" t="s">
         <v>444</v>
       </c>
@@ -6757,7 +6762,7 @@
         <v>27064</v>
       </c>
     </row>
-    <row r="271" spans="1:4" ht="57" x14ac:dyDescent="0.45">
+    <row r="271" spans="1:4" ht="60" x14ac:dyDescent="0.2">
       <c r="A271" s="11" t="s">
         <v>446</v>
       </c>
@@ -6771,7 +6776,7 @@
         <v>29864</v>
       </c>
     </row>
-    <row r="272" spans="1:4" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="272" spans="1:4" ht="75" x14ac:dyDescent="0.2">
       <c r="A272" s="11" t="s">
         <v>448</v>
       </c>
@@ -6785,7 +6790,7 @@
         <v>22078</v>
       </c>
     </row>
-    <row r="273" spans="1:4" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="273" spans="1:4" ht="75" x14ac:dyDescent="0.2">
       <c r="A273" s="11" t="s">
         <v>450</v>
       </c>
@@ -6799,7 +6804,7 @@
         <v>22856</v>
       </c>
     </row>
-    <row r="274" spans="1:4" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="274" spans="1:4" ht="75" x14ac:dyDescent="0.2">
       <c r="A274" s="11" t="s">
         <v>451</v>
       </c>
@@ -6813,7 +6818,7 @@
         <v>24975</v>
       </c>
     </row>
-    <row r="275" spans="1:4" ht="85.5" x14ac:dyDescent="0.45">
+    <row r="275" spans="1:4" ht="75" x14ac:dyDescent="0.2">
       <c r="A275" s="11" t="s">
         <v>453</v>
       </c>
@@ -6827,7 +6832,7 @@
         <v>23914</v>
       </c>
     </row>
-    <row r="276" spans="1:4" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="276" spans="1:4" ht="75" x14ac:dyDescent="0.2">
       <c r="A276" s="11" t="s">
         <v>455</v>
       </c>
@@ -6841,7 +6846,7 @@
         <v>24871</v>
       </c>
     </row>
-    <row r="277" spans="1:4" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="277" spans="1:4" ht="75" x14ac:dyDescent="0.2">
       <c r="A277" s="11" t="s">
         <v>457</v>
       </c>
@@ -6855,7 +6860,7 @@
         <v>27566</v>
       </c>
     </row>
-    <row r="278" spans="1:4" ht="85.5" x14ac:dyDescent="0.45">
+    <row r="278" spans="1:4" ht="90" x14ac:dyDescent="0.2">
       <c r="A278" s="11" t="s">
         <v>459</v>
       </c>
@@ -6869,7 +6874,7 @@
         <v>22430</v>
       </c>
     </row>
-    <row r="279" spans="1:4" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="279" spans="1:4" ht="75" x14ac:dyDescent="0.2">
       <c r="A279" s="11" t="s">
         <v>461</v>
       </c>
@@ -6883,7 +6888,7 @@
         <v>27065</v>
       </c>
     </row>
-    <row r="280" spans="1:4" ht="85.5" x14ac:dyDescent="0.45">
+    <row r="280" spans="1:4" ht="90" x14ac:dyDescent="0.2">
       <c r="A280" s="11" t="s">
         <v>462</v>
       </c>
@@ -6897,7 +6902,7 @@
         <v>27315</v>
       </c>
     </row>
-    <row r="281" spans="1:4" ht="57" x14ac:dyDescent="0.45">
+    <row r="281" spans="1:4" ht="60" x14ac:dyDescent="0.2">
       <c r="A281" s="11" t="s">
         <v>463</v>
       </c>
@@ -6911,7 +6916,7 @@
         <v>29426</v>
       </c>
     </row>
-    <row r="282" spans="1:4" ht="85.5" x14ac:dyDescent="0.45">
+    <row r="282" spans="1:4" ht="75" x14ac:dyDescent="0.2">
       <c r="A282" s="11" t="s">
         <v>465</v>
       </c>
@@ -6925,7 +6930,7 @@
         <v>27580</v>
       </c>
     </row>
-    <row r="283" spans="1:4" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="283" spans="1:4" ht="75" x14ac:dyDescent="0.2">
       <c r="A283" s="11" t="s">
         <v>467</v>
       </c>
@@ -6939,7 +6944,7 @@
         <v>26585</v>
       </c>
     </row>
-    <row r="284" spans="1:4" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="284" spans="1:4" ht="75" x14ac:dyDescent="0.2">
       <c r="A284" s="11" t="s">
         <v>468</v>
       </c>
@@ -6953,7 +6958,7 @@
         <v>22206</v>
       </c>
     </row>
-    <row r="285" spans="1:4" ht="57" x14ac:dyDescent="0.45">
+    <row r="285" spans="1:4" ht="60" x14ac:dyDescent="0.2">
       <c r="A285" s="11" t="s">
         <v>469</v>
       </c>
@@ -6967,7 +6972,7 @@
         <v>29932</v>
       </c>
     </row>
-    <row r="286" spans="1:4" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="286" spans="1:4" ht="75" x14ac:dyDescent="0.2">
       <c r="A286" s="11" t="s">
         <v>471</v>
       </c>
@@ -6981,7 +6986,7 @@
         <v>21510</v>
       </c>
     </row>
-    <row r="287" spans="1:4" ht="57" x14ac:dyDescent="0.45">
+    <row r="287" spans="1:4" ht="60" x14ac:dyDescent="0.2">
       <c r="A287" s="11" t="s">
         <v>473</v>
       </c>
@@ -6995,7 +7000,7 @@
         <v>26036</v>
       </c>
     </row>
-    <row r="288" spans="1:4" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="288" spans="1:4" ht="60" x14ac:dyDescent="0.2">
       <c r="A288" s="11" t="s">
         <v>475</v>
       </c>
@@ -7009,7 +7014,7 @@
         <v>21303</v>
       </c>
     </row>
-    <row r="289" spans="1:4" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="289" spans="1:4" ht="60" x14ac:dyDescent="0.2">
       <c r="A289" s="11" t="s">
         <v>477</v>
       </c>
@@ -7023,7 +7028,7 @@
         <v>26366</v>
       </c>
     </row>
-    <row r="290" spans="1:4" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="290" spans="1:4" ht="75" x14ac:dyDescent="0.2">
       <c r="A290" s="11" t="s">
         <v>479</v>
       </c>
@@ -7037,7 +7042,7 @@
         <v>28884</v>
       </c>
     </row>
-    <row r="291" spans="1:4" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="291" spans="1:4" ht="75" x14ac:dyDescent="0.2">
       <c r="A291" s="11" t="s">
         <v>480</v>
       </c>
@@ -7051,7 +7056,7 @@
         <v>29445</v>
       </c>
     </row>
-    <row r="292" spans="1:4" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="292" spans="1:4" ht="75" x14ac:dyDescent="0.2">
       <c r="A292" s="11" t="s">
         <v>481</v>
       </c>
@@ -7065,7 +7070,7 @@
         <v>28856</v>
       </c>
     </row>
-    <row r="293" spans="1:4" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="293" spans="1:4" ht="75" x14ac:dyDescent="0.2">
       <c r="A293" s="11" t="s">
         <v>483</v>
       </c>
@@ -7079,7 +7084,7 @@
         <v>23550</v>
       </c>
     </row>
-    <row r="294" spans="1:4" ht="57" x14ac:dyDescent="0.45">
+    <row r="294" spans="1:4" ht="60" x14ac:dyDescent="0.2">
       <c r="A294" s="11" t="s">
         <v>485</v>
       </c>
@@ -7093,7 +7098,7 @@
         <v>29639</v>
       </c>
     </row>
-    <row r="295" spans="1:4" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="295" spans="1:4" ht="75" x14ac:dyDescent="0.2">
       <c r="A295" s="11" t="s">
         <v>487</v>
       </c>
@@ -7107,7 +7112,7 @@
         <v>27684</v>
       </c>
     </row>
-    <row r="296" spans="1:4" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="296" spans="1:4" ht="60" x14ac:dyDescent="0.2">
       <c r="A296" s="11" t="s">
         <v>489</v>
       </c>
@@ -7121,7 +7126,7 @@
         <v>26539</v>
       </c>
     </row>
-    <row r="297" spans="1:4" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="297" spans="1:4" ht="75" x14ac:dyDescent="0.2">
       <c r="A297" s="11" t="s">
         <v>491</v>
       </c>
@@ -7135,7 +7140,7 @@
         <v>24934</v>
       </c>
     </row>
-    <row r="298" spans="1:4" ht="85.5" x14ac:dyDescent="0.45">
+    <row r="298" spans="1:4" ht="90" x14ac:dyDescent="0.2">
       <c r="A298" s="11" t="s">
         <v>492</v>
       </c>
@@ -7149,7 +7154,7 @@
         <v>25461</v>
       </c>
     </row>
-    <row r="299" spans="1:4" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="299" spans="1:4" ht="75" x14ac:dyDescent="0.2">
       <c r="A299" s="11" t="s">
         <v>493</v>
       </c>
@@ -7163,7 +7168,7 @@
         <v>26951</v>
       </c>
     </row>
-    <row r="300" spans="1:4" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="300" spans="1:4" ht="75" x14ac:dyDescent="0.2">
       <c r="A300" s="11" t="s">
         <v>495</v>
       </c>
@@ -7177,7 +7182,7 @@
         <v>23883</v>
       </c>
     </row>
-    <row r="301" spans="1:4" ht="85.5" x14ac:dyDescent="0.45">
+    <row r="301" spans="1:4" ht="90" x14ac:dyDescent="0.2">
       <c r="A301" s="11" t="s">
         <v>497</v>
       </c>
@@ -7191,7 +7196,7 @@
         <v>29609</v>
       </c>
     </row>
-    <row r="302" spans="1:4" ht="85.5" x14ac:dyDescent="0.45">
+    <row r="302" spans="1:4" ht="90" x14ac:dyDescent="0.2">
       <c r="A302" s="11" t="s">
         <v>498</v>
       </c>
@@ -7205,7 +7210,7 @@
         <v>25217</v>
       </c>
     </row>
-    <row r="303" spans="1:4" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="303" spans="1:4" ht="75" x14ac:dyDescent="0.2">
       <c r="A303" s="11" t="s">
         <v>500</v>
       </c>
@@ -7219,7 +7224,7 @@
         <v>25431</v>
       </c>
     </row>
-    <row r="304" spans="1:4" ht="57" x14ac:dyDescent="0.45">
+    <row r="304" spans="1:4" ht="60" x14ac:dyDescent="0.2">
       <c r="A304" s="11" t="s">
         <v>501</v>
       </c>
@@ -7233,7 +7238,7 @@
         <v>28821</v>
       </c>
     </row>
-    <row r="305" spans="1:4" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="305" spans="1:4" ht="75" x14ac:dyDescent="0.2">
       <c r="A305" s="11" t="s">
         <v>503</v>
       </c>
@@ -7247,7 +7252,7 @@
         <v>24640</v>
       </c>
     </row>
-    <row r="306" spans="1:4" ht="57" x14ac:dyDescent="0.45">
+    <row r="306" spans="1:4" ht="60" x14ac:dyDescent="0.2">
       <c r="A306" s="11" t="s">
         <v>504</v>
       </c>
@@ -7261,7 +7266,7 @@
         <v>25961</v>
       </c>
     </row>
-    <row r="307" spans="1:4" ht="57" x14ac:dyDescent="0.45">
+    <row r="307" spans="1:4" ht="60" x14ac:dyDescent="0.2">
       <c r="A307" s="11" t="s">
         <v>506</v>
       </c>
@@ -7275,7 +7280,7 @@
         <v>21562</v>
       </c>
     </row>
-    <row r="308" spans="1:4" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="308" spans="1:4" ht="75" x14ac:dyDescent="0.2">
       <c r="A308" s="11" t="s">
         <v>507</v>
       </c>
@@ -7289,7 +7294,7 @@
         <v>26173</v>
       </c>
     </row>
-    <row r="309" spans="1:4" ht="57" x14ac:dyDescent="0.45">
+    <row r="309" spans="1:4" ht="60" x14ac:dyDescent="0.2">
       <c r="A309" s="11" t="s">
         <v>509</v>
       </c>
@@ -7303,7 +7308,7 @@
         <v>24809</v>
       </c>
     </row>
-    <row r="310" spans="1:4" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="310" spans="1:4" ht="75" x14ac:dyDescent="0.2">
       <c r="A310" s="11" t="s">
         <v>511</v>
       </c>
@@ -7317,7 +7322,7 @@
         <v>26731</v>
       </c>
     </row>
-    <row r="311" spans="1:4" ht="85.5" x14ac:dyDescent="0.45">
+    <row r="311" spans="1:4" ht="90" x14ac:dyDescent="0.2">
       <c r="A311" s="11" t="s">
         <v>512</v>
       </c>
@@ -7331,7 +7336,7 @@
         <v>22618</v>
       </c>
     </row>
-    <row r="312" spans="1:4" ht="57" x14ac:dyDescent="0.45">
+    <row r="312" spans="1:4" ht="60" x14ac:dyDescent="0.2">
       <c r="A312" s="11" t="s">
         <v>513</v>
       </c>
@@ -7345,7 +7350,7 @@
         <v>26081</v>
       </c>
     </row>
-    <row r="313" spans="1:4" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="313" spans="1:4" ht="75" x14ac:dyDescent="0.2">
       <c r="A313" s="11" t="s">
         <v>515</v>
       </c>
@@ -7359,7 +7364,7 @@
         <v>22608</v>
       </c>
     </row>
-    <row r="314" spans="1:4" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="314" spans="1:4" ht="75" x14ac:dyDescent="0.2">
       <c r="A314" s="11" t="s">
         <v>516</v>
       </c>
@@ -7373,7 +7378,7 @@
         <v>21703</v>
       </c>
     </row>
-    <row r="315" spans="1:4" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="315" spans="1:4" ht="60" x14ac:dyDescent="0.2">
       <c r="A315" s="11" t="s">
         <v>518</v>
       </c>
@@ -7387,7 +7392,7 @@
         <v>22254</v>
       </c>
     </row>
-    <row r="316" spans="1:4" ht="57" x14ac:dyDescent="0.45">
+    <row r="316" spans="1:4" ht="60" x14ac:dyDescent="0.2">
       <c r="A316" s="11" t="s">
         <v>520</v>
       </c>
@@ -7401,7 +7406,7 @@
         <v>26814</v>
       </c>
     </row>
-    <row r="317" spans="1:4" ht="57" x14ac:dyDescent="0.45">
+    <row r="317" spans="1:4" ht="60" x14ac:dyDescent="0.2">
       <c r="A317" s="11" t="s">
         <v>522</v>
       </c>
@@ -7415,7 +7420,7 @@
         <v>27073</v>
       </c>
     </row>
-    <row r="318" spans="1:4" ht="57" x14ac:dyDescent="0.45">
+    <row r="318" spans="1:4" ht="60" x14ac:dyDescent="0.2">
       <c r="A318" s="11" t="s">
         <v>524</v>
       </c>
@@ -7429,7 +7434,7 @@
         <v>29203</v>
       </c>
     </row>
-    <row r="319" spans="1:4" ht="85.5" x14ac:dyDescent="0.45">
+    <row r="319" spans="1:4" ht="90" x14ac:dyDescent="0.2">
       <c r="A319" s="11" t="s">
         <v>525</v>
       </c>
@@ -7443,7 +7448,7 @@
         <v>21050</v>
       </c>
     </row>
-    <row r="320" spans="1:4" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="320" spans="1:4" ht="75" x14ac:dyDescent="0.2">
       <c r="A320" s="11" t="s">
         <v>526</v>
       </c>
@@ -7457,7 +7462,7 @@
         <v>21362</v>
       </c>
     </row>
-    <row r="321" spans="1:4" ht="85.5" x14ac:dyDescent="0.45">
+    <row r="321" spans="1:4" ht="90" x14ac:dyDescent="0.2">
       <c r="A321" s="11" t="s">
         <v>527</v>
       </c>
@@ -7471,7 +7476,7 @@
         <v>22884</v>
       </c>
     </row>
-    <row r="322" spans="1:4" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="322" spans="1:4" ht="75" x14ac:dyDescent="0.2">
       <c r="A322" s="11" t="s">
         <v>528</v>
       </c>
@@ -7485,7 +7490,7 @@
         <v>21828</v>
       </c>
     </row>
-    <row r="323" spans="1:4" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="323" spans="1:4" ht="75" x14ac:dyDescent="0.2">
       <c r="A323" s="11" t="s">
         <v>530</v>
       </c>
@@ -7499,7 +7504,7 @@
         <v>26114</v>
       </c>
     </row>
-    <row r="324" spans="1:4" ht="85.5" x14ac:dyDescent="0.45">
+    <row r="324" spans="1:4" ht="90" x14ac:dyDescent="0.2">
       <c r="A324" s="11" t="s">
         <v>532</v>
       </c>
@@ -7513,7 +7518,7 @@
         <v>26426</v>
       </c>
     </row>
-    <row r="325" spans="1:4" ht="85.5" x14ac:dyDescent="0.45">
+    <row r="325" spans="1:4" ht="90" x14ac:dyDescent="0.2">
       <c r="A325" s="11" t="s">
         <v>534</v>
       </c>
@@ -7527,7 +7532,7 @@
         <v>25671</v>
       </c>
     </row>
-    <row r="326" spans="1:4" ht="85.5" x14ac:dyDescent="0.45">
+    <row r="326" spans="1:4" ht="90" x14ac:dyDescent="0.2">
       <c r="A326" s="11" t="s">
         <v>535</v>
       </c>
@@ -7541,7 +7546,7 @@
         <v>26515</v>
       </c>
     </row>
-    <row r="327" spans="1:4" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="327" spans="1:4" ht="75" x14ac:dyDescent="0.2">
       <c r="A327" s="11" t="s">
         <v>537</v>
       </c>
@@ -7555,7 +7560,7 @@
         <v>25965</v>
       </c>
     </row>
-    <row r="328" spans="1:4" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="328" spans="1:4" ht="75" x14ac:dyDescent="0.2">
       <c r="A328" s="11" t="s">
         <v>538</v>
       </c>
@@ -7569,7 +7574,7 @@
         <v>234823</v>
       </c>
     </row>
-    <row r="329" spans="1:4" ht="85.5" x14ac:dyDescent="0.45">
+    <row r="329" spans="1:4" ht="90" x14ac:dyDescent="0.2">
       <c r="A329" s="11" t="s">
         <v>539</v>
       </c>
@@ -7583,7 +7588,7 @@
         <v>23482</v>
       </c>
     </row>
-    <row r="330" spans="1:4" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="330" spans="1:4" ht="75" x14ac:dyDescent="0.2">
       <c r="A330" s="11" t="s">
         <v>541</v>
       </c>
@@ -7597,7 +7602,7 @@
         <v>3578</v>
       </c>
     </row>
-    <row r="331" spans="1:4" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="331" spans="1:4" ht="75" x14ac:dyDescent="0.2">
       <c r="A331" s="11" t="s">
         <v>542</v>
       </c>
@@ -7611,7 +7616,7 @@
         <v>19389</v>
       </c>
     </row>
-    <row r="332" spans="1:4" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="332" spans="1:4" ht="75" x14ac:dyDescent="0.2">
       <c r="A332" s="11" t="s">
         <v>544</v>
       </c>
@@ -7625,7 +7630,7 @@
         <v>52987</v>
       </c>
     </row>
-    <row r="333" spans="1:4" ht="85.5" x14ac:dyDescent="0.45">
+    <row r="333" spans="1:4" ht="90" x14ac:dyDescent="0.2">
       <c r="A333" s="11" t="s">
         <v>546</v>
       </c>
@@ -7639,7 +7644,7 @@
         <v>9843</v>
       </c>
     </row>
-    <row r="334" spans="1:4" ht="57" x14ac:dyDescent="0.45">
+    <row r="334" spans="1:4" ht="60" x14ac:dyDescent="0.2">
       <c r="A334" s="11" t="s">
         <v>547</v>
       </c>
@@ -7653,7 +7658,7 @@
         <v>67453</v>
       </c>
     </row>
-    <row r="335" spans="1:4" ht="57" x14ac:dyDescent="0.45">
+    <row r="335" spans="1:4" ht="60" x14ac:dyDescent="0.2">
       <c r="A335" s="11" t="s">
         <v>549</v>
       </c>
@@ -7667,7 +7672,7 @@
         <v>31632</v>
       </c>
     </row>
-    <row r="336" spans="1:4" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="336" spans="1:4" ht="60" x14ac:dyDescent="0.2">
       <c r="A336" s="11" t="s">
         <v>551</v>
       </c>
@@ -7681,7 +7686,7 @@
         <v>54784</v>
       </c>
     </row>
-    <row r="337" spans="1:4" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="337" spans="1:4" ht="60" x14ac:dyDescent="0.2">
       <c r="A337" s="11" t="s">
         <v>553</v>
       </c>
@@ -7695,7 +7700,7 @@
         <v>38279</v>
       </c>
     </row>
-    <row r="338" spans="1:4" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="338" spans="1:4" ht="75" x14ac:dyDescent="0.2">
       <c r="A338" s="11" t="s">
         <v>555</v>
       </c>
@@ -7709,7 +7714,7 @@
         <v>74353</v>
       </c>
     </row>
-    <row r="339" spans="1:4" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="339" spans="1:4" ht="75" x14ac:dyDescent="0.2">
       <c r="A339" s="11" t="s">
         <v>556</v>
       </c>
@@ -7723,7 +7728,7 @@
         <v>7364</v>
       </c>
     </row>
-    <row r="340" spans="1:4" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="340" spans="1:4" ht="60" x14ac:dyDescent="0.2">
       <c r="A340" s="11" t="s">
         <v>558</v>
       </c>
@@ -7737,7 +7742,7 @@
         <v>34632</v>
       </c>
     </row>
-    <row r="341" spans="1:4" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="341" spans="1:4" ht="75" x14ac:dyDescent="0.2">
       <c r="A341" s="11" t="s">
         <v>560</v>
       </c>
@@ -7751,7 +7756,7 @@
         <v>78864</v>
       </c>
     </row>
-    <row r="342" spans="1:4" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="342" spans="1:4" ht="75" x14ac:dyDescent="0.2">
       <c r="A342" s="11" t="s">
         <v>561</v>
       </c>
@@ -7765,7 +7770,7 @@
         <v>54643</v>
       </c>
     </row>
-    <row r="343" spans="1:4" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="343" spans="1:4" ht="75" x14ac:dyDescent="0.2">
       <c r="A343" s="11" t="s">
         <v>563</v>
       </c>
@@ -7779,7 +7784,7 @@
         <v>62747</v>
       </c>
     </row>
-    <row r="344" spans="1:4" ht="85.5" x14ac:dyDescent="0.45">
+    <row r="344" spans="1:4" ht="90" x14ac:dyDescent="0.2">
       <c r="A344" s="11" t="s">
         <v>565</v>
       </c>
@@ -7793,7 +7798,7 @@
         <v>95688</v>
       </c>
     </row>
-    <row r="345" spans="1:4" ht="85.5" x14ac:dyDescent="0.45">
+    <row r="345" spans="1:4" ht="75" x14ac:dyDescent="0.2">
       <c r="A345" s="11" t="s">
         <v>567</v>
       </c>
@@ -7807,7 +7812,7 @@
         <v>4584</v>
       </c>
     </row>
-    <row r="346" spans="1:4" ht="57" x14ac:dyDescent="0.45">
+    <row r="346" spans="1:4" ht="60" x14ac:dyDescent="0.2">
       <c r="A346" s="11" t="s">
         <v>569</v>
       </c>
@@ -7821,7 +7826,7 @@
         <v>845643</v>
       </c>
     </row>
-    <row r="347" spans="1:4" ht="57" x14ac:dyDescent="0.45">
+    <row r="347" spans="1:4" ht="60" x14ac:dyDescent="0.2">
       <c r="A347" s="11" t="s">
         <v>571</v>
       </c>
@@ -7835,7 +7840,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="348" spans="1:4" ht="57" x14ac:dyDescent="0.45">
+    <row r="348" spans="1:4" ht="60" x14ac:dyDescent="0.2">
       <c r="A348" s="11" t="s">
         <v>573</v>
       </c>
@@ -7849,7 +7854,7 @@
         <v>42562</v>
       </c>
     </row>
-    <row r="349" spans="1:4" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="349" spans="1:4" ht="75" x14ac:dyDescent="0.2">
       <c r="A349" s="11" t="s">
         <v>575</v>
       </c>
@@ -7863,7 +7868,7 @@
         <v>6542</v>
       </c>
     </row>
-    <row r="350" spans="1:4" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="350" spans="1:4" ht="75" x14ac:dyDescent="0.2">
       <c r="A350" s="11" t="s">
         <v>577</v>
       </c>
@@ -7877,7 +7882,7 @@
         <v>32522</v>
       </c>
     </row>
-    <row r="351" spans="1:4" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="351" spans="1:4" ht="60" x14ac:dyDescent="0.2">
       <c r="A351" s="11" t="s">
         <v>578</v>
       </c>
@@ -7891,7 +7896,7 @@
         <v>246364</v>
       </c>
     </row>
-    <row r="352" spans="1:4" ht="85.5" x14ac:dyDescent="0.45">
+    <row r="352" spans="1:4" ht="90" x14ac:dyDescent="0.2">
       <c r="A352" s="11" t="s">
         <v>580</v>
       </c>

</xml_diff>